<commit_message>
Committing in preparation for implementing multithreading...
</commit_message>
<xml_diff>
--- a/docs/counts and scores.xlsx
+++ b/docs/counts and scores.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>uc</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>beta</t>
+  </si>
+  <si>
+    <t>gamma</t>
   </si>
 </sst>
 </file>
@@ -144,12 +147,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -222,37 +226,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.89595845984076194</c:v>
+                  <c:v>7.1277811011064909E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41205319475393282</c:v>
+                  <c:v>1.7736200269505303E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22557774482832002</c:v>
+                  <c:v>7.552162701187025E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13788178155275871</c:v>
+                  <c:v>1.1074271680528042E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.093907957118165E-2</c:v>
+                  <c:v>2.775579465207388E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.3412123590278646E-2</c:v>
+                  <c:v>9.4008778546387652E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6138182948722822E-2</c:v>
+                  <c:v>3.8627071624482668E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.4714847540041373E-2</c:v>
+                  <c:v>1.8157763921595928E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.6838300568090018E-2</c:v>
+                  <c:v>9.4253062960327366E-12</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1219048132590373E-2</c:v>
+                  <c:v>5.2793486056596163E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.7094964806248742E-2</c:v>
+                  <c:v>3.1407712882628949E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -279,37 +283,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.85133992252078472</c:v>
+                  <c:v>7.1554175279993273E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.52037165862036061</c:v>
+                  <c:v>1.5583542199414839E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.34320792157561103</c:v>
+                  <c:v>7.9159784279003844E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.23932002877904782</c:v>
+                  <c:v>1.2393479666320925E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17412744828489032</c:v>
+                  <c:v>3.2141804810531992E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13101529868361958</c:v>
+                  <c:v>1.1117209769583951E-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.10128887822518379</c:v>
+                  <c:v>4.6332119348368309E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.0081582546685598E-2</c:v>
+                  <c:v>2.200388571220797E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.4517118143563507E-2</c:v>
+                  <c:v>1.1510445365997865E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.2817314407941747E-2</c:v>
+                  <c:v>6.4864162138221395E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.3840511427054932E-2</c:v>
+                  <c:v>3.8776839725647936E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -336,37 +340,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.82317125399304369</c:v>
+                  <c:v>1.5741960558485099E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57400006180305885</c:v>
+                  <c:v>1.2899088739809705E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.41763811657157218</c:v>
+                  <c:v>7.6682831282530988E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.31423525195617802</c:v>
+                  <c:v>1.2762469564477751E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.2429375537761429</c:v>
+                  <c:v>3.419251086247638E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1920726550368384</c:v>
+                  <c:v>1.2067566792842419E-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.15474187426223007</c:v>
+                  <c:v>5.0988826720121202E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1266803363224582</c:v>
+                  <c:v>2.4457926742693949E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.10514981298051038</c:v>
+                  <c:v>1.2891206680328642E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.8334621168559044E-2</c:v>
+                  <c:v>7.3076832507279356E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.4996814370496073E-2</c:v>
+                  <c:v>4.3895473088157421E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -393,37 +397,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.80274156176023015</c:v>
+                  <c:v>5.0805263425290857E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.60399107961256404</c:v>
+                  <c:v>1.0478829777383199E-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.46694988697242207</c:v>
+                  <c:v>7.173678459514149E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.36918254574419912</c:v>
+                  <c:v>1.2641975308641976E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.29742911119962417</c:v>
+                  <c:v>3.4935147673396774E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.24349207361290753</c:v>
+                  <c:v>1.2571481127930194E-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2021082888307339</c:v>
+                  <c:v>5.383016257400223E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16978783530692243</c:v>
+                  <c:v>2.6072533413223757E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.14415125800543849</c:v>
+                  <c:v>1.384403258095006E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.12353634864011014</c:v>
+                  <c:v>7.8934984392986608E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.10675686255873086</c:v>
+                  <c:v>4.7636938529609064E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -450,37 +454,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.7867934421967725</c:v>
+                  <c:v>2.0593630529182679E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.62205905616206081</c:v>
+                  <c:v>8.4747450737377282E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.50115714927691979</c:v>
+                  <c:v>6.5899617693384578E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.41027521815599882</c:v>
+                  <c:v>1.2253007990231857E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.34054505783620453</c:v>
+                  <c:v>3.4875494130607935E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.28608627844503981</c:v>
+                  <c:v>1.2787024314771518E-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.2428895854723537</c:v>
+                  <c:v>5.5464634477845478E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.20815421888883184</c:v>
+                  <c:v>2.711918423596073E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1798813999406158</c:v>
+                  <c:v>1.4504017326521389E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1566173939180287</c:v>
+                  <c:v>8.3169657308462547E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.13728683268692438</c:v>
+                  <c:v>5.0423901194369781E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -507,37 +511,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.773758913061102</c:v>
+                  <c:v>9.7107978751659442E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.63344223925433707</c:v>
+                  <c:v>6.8648563583535223E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.52578272938908455</c:v>
+                  <c:v>5.9923531206993966E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.44170138682190874</c:v>
+                  <c:v>1.1717533928321049E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.37500808263458074</c:v>
+                  <c:v>3.4305583235107347E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.32137859828775811</c:v>
+                  <c:v>1.2806961942253445E-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.27772692996354359</c:v>
+                  <c:v>5.625118359524747E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.24180859169488719</c:v>
+                  <c:v>2.775807343782481E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.21196327457505579</c:v>
+                  <c:v>1.4950738840146333E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.18694397710859695</c:v>
+                  <c:v>8.6210348293517169E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.16580115773109833</c:v>
+                  <c:v>5.2503961286370369E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -564,37 +568,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.76276520578267581</c:v>
+                  <c:v>5.1002249826599734E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64078645109772414</c:v>
+                  <c:v>5.5851778781637985E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54403292716231055</c:v>
+                  <c:v>5.417333487789897E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46623138980228152</c:v>
+                  <c:v>1.1107607757728456E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.40290490167140708</c:v>
+                  <c:v>3.340869456212092E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.35079733489625498</c:v>
+                  <c:v>1.2690991828852465E-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.30750004082003379</c:v>
+                  <c:v>5.6423361435155033E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.27120396543787867</c:v>
+                  <c:v>2.8093904802394015E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.24053158676914244</c:v>
+                  <c:v>1.5236274671448739E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.2144208043939223</c:v>
+                  <c:v>8.8338010142549864E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1920433398045554</c:v>
+                  <c:v>5.4038877366376386E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -621,37 +625,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.7532776949250386</c:v>
+                  <c:v>2.9038879447843412E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6455522985416281</c:v>
+                  <c:v>4.5698445331918777E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.55786931351397562</c:v>
+                  <c:v>4.88174719772738E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.48572024710860967</c:v>
+                  <c:v>1.0467283786331982E-9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.42577004143200203</c:v>
+                  <c:v>3.2305611447847429E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.37551384804071836</c:v>
+                  <c:v>1.2479749151131164E-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.33304432542934098</c:v>
+                  <c:v>5.6142677228610724E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.29689087041166873</c:v>
+                  <c:v>2.8199662377501052E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.26590663379189533</c:v>
+                  <c:v>1.5397064023699039E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.23918787257892171</c:v>
+                  <c:v>8.9749525487978353E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.21601555852892354</c:v>
+                  <c:v>5.5142027517397216E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -678,37 +682,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.7449457381771869</c:v>
+                  <c:v>1.7603896062074554E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64860213541905876</c:v>
+                  <c:v>3.7623354692431818E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.56854817091556775</c:v>
+                  <c:v>4.3921185432816873E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.50143901797072232</c:v>
+                  <c:v>9.823860162910882E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.44472772536980271</c:v>
+                  <c:v>3.1078347045104637E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.39645053645946332</c:v>
+                  <c:v>1.2201922126836812E-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.35507601654693277</c:v>
+                  <c:v>5.5525447070035634E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.31939736060938945</c:v>
+                  <c:v>2.81284813169556E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.28845442078981631</c:v>
+                  <c:v>1.5459795458345003E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.26147650889852803</c:v>
+                  <c:v>9.0589556030578899E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.23783992987563579</c:v>
+                  <c:v>5.5896845019651346E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -735,37 +739,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.73752724891279675</c:v>
+                  <c:v>1.1220524896313387E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65047248120758128</c:v>
+                  <c:v>3.1172193932805887E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.57690593794196887</c:v>
+                  <c:v>3.9495067840919939E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5142802113215702</c:v>
+                  <c:v>9.194188094111114E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46060870658867048</c:v>
+                  <c:v>2.9783597742397527E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4143259423399569</c:v>
+                  <c:v>1.1878269350919362E-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.37418640369426304</c:v>
+                  <c:v>5.4657843559496194E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.33919034503743473</c:v>
+                  <c:v>2.7920256509994524E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.30852870193973403</c:v>
+                  <c:v>1.5444665846866091E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.28154173237033125</c:v>
+                  <c:v>9.0968089365131296E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.25768764288415691</c:v>
+                  <c:v>5.636693683808007E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -792,37 +796,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.73084825842593237</c:v>
+                  <c:v>7.4511745618788787E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6515114025834452</c:v>
+                  <c:v>2.5989704947756442E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5835181246825949</c:v>
+                  <c:v>3.5521386117832702E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.52488520825434881</c:v>
+                  <c:v>8.5884320665167032E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.47403478362901474</c:v>
+                  <c:v>2.8460925866550344E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.42970033179037287</c:v>
+                  <c:v>1.1524065370859347E-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.39085689651845823</c:v>
+                  <c:v>5.3605015652055841E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.35666868937267632</c:v>
+                  <c:v>2.7605625130252493E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.32644934405011089</c:v>
+                  <c:v>1.5367334192817319E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.29963147499141563</c:v>
+                  <c:v>9.0970912203013103E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.27574315219358198</c:v>
+                  <c:v>5.6602100746585705E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -849,37 +853,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.72477966367769564</c:v>
+                  <c:v>5.1200000000000003E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65195254203100761</c:v>
+                  <c:v>2.1801215842470901E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58879194410122582</c:v>
+                  <c:v>3.1968668679159576E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.53372474441411333</c:v>
+                  <c:v>8.0124077569734154E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.48547785925047182</c:v>
+                  <c:v>2.7137996799972411E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.44301316753186964</c:v>
+                  <c:v>1.1150675100201012E-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.40547814331756116</c:v>
+                  <c:v>5.2416949440075422E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.37216804497659456</c:v>
+                  <c:v>2.720851563604588E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.3424966948833032</c:v>
+                  <c:v>1.5240166693117275E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.31597370786794782</c:v>
+                  <c:v>9.0666257437081505E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.29218660536270025</c:v>
+                  <c:v>5.6642130794262971E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -906,37 +910,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.71922309332486423</c:v>
+                  <c:v>3.6212879647952505E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65195722446152593</c:v>
+                  <c:v>1.8395071572117217E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.59302252887282747</c:v>
+                  <c:v>2.8799844209532715E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.54115091744723187</c:v>
+                  <c:v>7.4690804848943912E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.49530100986290276</c:v>
+                  <c:v>2.5834060976335819E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.45461194777949454</c:v>
+                  <c:v>1.0766611597843494E-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.41836770155462916</c:v>
+                  <c:v>5.1132409749139679E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.38596925426520845</c:v>
+                  <c:v>2.6747857925964039E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.35691275371954456</c:v>
+                  <c:v>1.507306918362175E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.33077222508506426</c:v>
+                  <c:v>9.0109232685593169E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.30718579699177939</c:v>
+                  <c:v>5.651934442654422E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -963,37 +967,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.71410191909521781</c:v>
+                  <c:v>2.6254817841431038E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65163950753054223</c:v>
+                  <c:v>1.5608030981867192E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.59642827119093744</c:v>
+                  <c:v>2.5976743038292667E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.54743158741372244</c:v>
+                  <c:v>6.9595470063314969E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.50378723239312873</c:v>
+                  <c:v>2.4562337257015717E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.46477388592034746</c:v>
+                  <c:v>1.037827077934207E-10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.42978482261901124</c:v>
+                  <c:v>4.9781688021627458E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.39830709495236305</c:v>
+                  <c:v>2.6238774689851504E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.36990494706427146</c:v>
+                  <c:v>1.487406563834284E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.34420651298245203</c:v>
+                  <c:v>8.9344888870809753E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.32089308284436174</c:v>
+                  <c:v>5.6260328476689453E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1020,37 +1024,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.70935532069514695</c:v>
+                  <c:v>1.9447884999558742E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65108166062134665</c:v>
+                  <c:v>1.3313783759094749E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.59917373313436306</c:v>
+                  <c:v>2.3462513199744615E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55277364407867324</c:v>
+                  <c:v>6.4836890075380893E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.51115979138624024</c:v>
+                  <c:v>2.3331681537359964E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.47372210661797171</c:v>
+                  <c:v>9.9904553608291998E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.43994232840028497</c:v>
+                  <c:v>4.8388574128947406E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.40937818208127802</c:v>
+                  <c:v>2.569343708069049E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.38165061363606145</c:v>
+                  <c:v>1.4649713102793827E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.35643342794550431</c:v>
+                  <c:v>8.8410416233160572E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.33344483205307562</c:v>
+                  <c:v>5.5887185574799863E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1077,37 +1081,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.70493424068343191</c:v>
+                  <c:v>1.4678689048907796E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65034404465629492</c:v>
+                  <c:v>1.1414148604430704E-8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.601384906384</c:v>
+                  <c:v>2.1222832384628993E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55733907388895809</c:v>
+                  <c:v>6.0406127773283111E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.51759680717814449</c:v>
+                  <c:v>2.2147775790802882E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.48163776544108811</c:v>
+                  <c:v>9.6067564938864846E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.44901598760433586</c:v>
+                  <c:v>4.6971804956504952E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4193477016566946</c:v>
+                  <c:v>2.512169492339436E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.39230137520137004</c:v>
+                  <c:v>1.4405407210634934E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.36758955256988063</c:v>
+                  <c:v>8.7336758784481444E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.34496212431913259</c:v>
+                  <c:v>5.5418448626566281E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1134,37 +1138,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.70079855159577498</c:v>
+                  <c:v>1.1264030050525835E-7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64947159727968862</c:v>
+                  <c:v>9.8324046566225758E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60315962195005268</c:v>
+                  <c:v>1.9226426220274217E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5612562683763429</c:v>
+                  <c:v>5.6289469187632616E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.52324185461937778</c:v>
+                  <c:v>2.1013987277088866E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.48866916814234079</c:v>
+                  <c:v>9.22983656640531E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45715187164109583</c:v>
+                  <c:v>4.5546149406009183E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.42835499076896194</c:v>
+                  <c:v>2.4531550666467651E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.40198707102882753</c:v>
+                  <c:v>1.4145612131604462E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.37779368029300103</c:v>
+                  <c:v>8.6149828463878401E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.355552001803769</c:v>
+                  <c:v>5.4869767505563733E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1191,37 +1195,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.69691502481948309</c:v>
+                  <c:v>8.7718711095448732E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64849819512284956</c:v>
+                  <c:v>8.5082609988308973E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60457480379688433</c:v>
+                  <c:v>1.7445192563537052E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5646281233869419</c:v>
+                  <c:v>5.2470443919580889E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.52821176414460025</c:v>
+                  <c:v>1.9931996259281205E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4949386831600962</c:v>
+                  <c:v>8.8616417394957229E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.46447212211822392</c:v>
+                  <c:v>4.4123234257928975E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.43651809984694823</c:v>
+                  <c:v>2.3929522124998264E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.41081916485153885</c:v>
+                  <c:v>1.3874036887413698E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.38714917401783949</c:v>
+                  <c:v>8.4871436058576603E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.3653089110318512</c:v>
+                  <c:v>5.4254435029156751E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1248,37 +1252,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.69325584403428708</c:v>
+                  <c:v>6.9216441571272889E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64744965186411763</c:v>
+                  <c:v>7.3940626912577473E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6056916200959146</c:v>
+                  <c:v>1.5854109069669731E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.56753793308039824</c:v>
+                  <c:v>4.8931193412882969E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.53260243567418941</c:v>
+                  <c:v>1.8902258526945462E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5005480245705185</c:v>
+                  <c:v>8.5035635453767495E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.47107948443431674</c:v>
+                  <c:v>4.2712181324877666E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.44393750072833837</c:v>
+                  <c:v>2.3320924259564187E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.41889363542797609</c:v>
+                  <c:v>1.3593772702480002E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.39574609424648566</c:v>
+                  <c:v>8.3520016885860879E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.37431614731721402</c:v>
+                  <c:v>5.3583796779736705E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1305,37 +1309,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.68979749727836415</c:v>
+                  <c:v>5.5267859485853923E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64634581833475013</c:v>
+                  <c:v>6.45192308021738E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60655920435920663</c:v>
+                  <c:v>1.4431029011925225E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57005374213646276</c:v>
+                  <c:v>4.5653390868065248E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.53649322295480373</c:v>
+                  <c:v>1.7924348402111083E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5055823240577888</c:v>
+                  <c:v>8.1565629424673608E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.47706088669065017</c:v>
+                  <c:v>4.1320104644700577E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.45069909556563592</c:v>
+                  <c:v>2.2710090848005329E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.42629340252289766</c:v>
+                  <c:v>1.3307401465162417E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.40366306713552463</c:v>
+                  <c:v>8.2111204636147892E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.38264721079844616</c:v>
+                  <c:v>5.2867575194940816E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1362,37 +1366,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.68651993776308051</c:v>
+                  <c:v>4.4605863380935203E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64520207880874014</c:v>
+                  <c:v>5.6515483129944283E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60721738518888235</c:v>
+                  <c:v>1.3156427132096505E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57223160270554141</c:v>
+                  <c:v>4.2618851106657757E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.53995027671876117</c:v>
+                  <c:v>1.6997214280495356E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.51011329613648237</c:v>
+                  <c:v>7.82126631114527E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.48249027970486097</c:v>
+                  <c:v>3.9952502224580523E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.45687666057247966</c:v>
+                  <c:v>2.2100550773376159E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.43309035202934076</c:v>
+                  <c:v>1.3017082387567794E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.41096889880084098</c:v>
+                  <c:v>8.0658290822293934E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.39036703549100099</c:v>
+                  <c:v>5.2114129201546373E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1419,37 +1423,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.68340593899316804</c:v>
+                  <c:v>3.6353287242794937E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64403043342854871</c:v>
+                  <c:v>4.9685795025359601E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60769871691967825</c:v>
+                  <c:v>1.2013131295908181E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5741180418123436</c:v>
+                  <c:v>3.9809925326293978E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.54302912054174501</c:v>
+                  <c:v>1.6119369553203056E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.51420171892060484</c:v>
+                  <c:v>7.4980402262009041E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.48743090352300472</c:v>
+                  <c:v>3.8613567252660141E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4625338355465769</c:v>
+                  <c:v>2.1495169536956902E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.43934702290963223</c:v>
+                  <c:v>1.2724621955897575E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.41772395793666922</c:v>
+                  <c:v>7.917259665404074E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.39753308059618986</c:v>
+                  <c:v>5.1330664589438755E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1476,37 +1480,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.68044059271095747</c:v>
+                  <c:v>2.9892321136954355E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64284029203977966</c:v>
+                  <c:v>4.3833230099795418E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60803000953114239</c:v>
+                  <c:v>1.0986060019876761E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57575195183697414</c:v>
+                  <c:v>3.7209746521479938E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.54577665488582661</c:v>
+                  <c:v>1.5289035409654088E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.51789939396858053</c:v>
+                  <c:v>7.1870500113568406E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.49193710691006448</c:v>
+                  <c:v>3.7306437078068333E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.46772574898420077</c:v>
+                  <c:v>2.0896263780109643E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.44511801235024978</c:v>
+                  <c:v>1.2431530897993464E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.42398135425163769</c:v>
+                  <c:v>7.7663776911241313E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.40419628756352449</c:v>
+                  <c:v>5.052340618807899E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1533,37 +1537,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.67761091340048019</c:v>
+                  <c:v>2.4780932222490048E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64163906363305778</c:v>
+                  <c:v>3.8797728216316997E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60823349478263178</c:v>
+                  <c:v>1.0061976466623099E-9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57716605413475186</c:v>
+                  <c:v>3.4802371470880281E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.54823273049624899</c:v>
+                  <c:v>1.4504247576641873E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.52125070641579085</c:v>
+                  <c:v>6.888305791028675E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.49605581664010062</c:v>
+                  <c:v>3.6033393605536137E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4725003506665077</c:v>
+                  <c:v>2.0305694618248362E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.45045114766654443</c:v>
+                  <c:v>1.2139070941082829E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.42978794057689951</c:v>
+                  <c:v>7.6140070344535117E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.4104019131529088</c:v>
+                  <c:v>4.9697740036630793E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1590,37 +1594,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.67490552337743748</c:v>
+                  <c:v>2.0698277612564798E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64043259896549243</c:v>
+                  <c:v>3.4448537390878475E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.6083277246026112</c:v>
+                  <c:v>9.2292638425754063E-10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57838804314802084</c:v>
+                  <c:v>3.2572851498679879E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55043139423545817</c:v>
+                  <c:v>1.376293588722063E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5242938759506609</c:v>
+                  <c:v>6.6016988298575923E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.49982773092840471</c:v>
+                  <c:v>3.479602541634079E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.47689950892958655</c:v>
+                  <c:v>1.9724944175700292E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.45538846572491465</c:v>
+                  <c:v>1.1848293453928942E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.43518516451290462</c:v>
+                  <c:v>7.4608507552135507E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.4161902513941097</c:v>
+                  <c:v>4.8858331706550357E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1647,37 +1651,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.67231439957775063</c:v>
+                  <c:v>1.7408389165209195E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.63922552634935847</c:v>
+                  <c:v>3.0678323154828189E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60832827003881673</c:v>
+                  <c:v>8.4777238020190374E-10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.57944148878357271</c:v>
+                  <c:v>3.0507254694116002E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55240188342715801</c:v>
+                  <c:v>1.3062983296552388E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.52706196682777795</c:v>
+                  <c:v>6.3270302780069004E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.50328829432931099</c:v>
+                  <c:v>3.3595359500032078E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4809599180700932</c:v>
+                  <c:v>1.9155178682986172E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.45996703365596187</c:v>
+                  <c:v>1.1560071576148503E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.44020979257958059</c:v>
+                  <c:v>7.307508469707434E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.42159725781010382</c:v>
+                  <c:v>4.8009225472008313E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1704,37 +1708,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.66982866811966113</c:v>
+                  <c:v>1.4735602485365581E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.63802150878243458</c:v>
+                  <c:v>2.7398558795006509E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60824826999934656</c:v>
+                  <c:v>7.798397562493428E-10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5803465540640621</c:v>
+                  <c:v>2.8592655597771789E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55416942541451741</c:v>
+                  <c:v>1.2402269303964103E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.52958370867636184</c:v>
+                  <c:v>6.0640339445948893E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.50646849851818465</c:v>
+                  <c:v>3.2431968688936589E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.48471385200953715</c:v>
+                  <c:v>1.8597300740708445E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.46421963862344223</c:v>
+                  <c:v>1.1275127076134366E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.44489452674193325</c:v>
+                  <c:v>7.1544909534447495E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.42665508863615059</c:v>
+                  <c:v>4.7153927953169862E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1761,37 +1765,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.66744043624217186</c:v>
+                  <c:v>1.2547671765709797E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.63682344253371237</c:v>
+                  <c:v>2.4535898782109877E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60809886570024529</c:v>
+                  <c:v>7.1834084122719941E-10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5811205702994896</c:v>
+                  <c:v>2.6817103653694172E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55575588500113304</c:v>
+                  <c:v>1.1778701521239204E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.53188416769063163</c:v>
+                  <c:v>5.8123943521145787E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.50939554355879468</c:v>
+                  <c:v>3.1306059546622584E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.48818979297830062</c:v>
+                  <c:v>1.8051992788240728E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.46817536938421667</c:v>
+                  <c:v>1.0994052909619213E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.44926853024511365</c:v>
+                  <c:v>7.0022324809109118E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.43139256662846093</c:v>
+                  <c:v>4.629547906328524E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1818,37 +1822,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.66514265376588477</c:v>
+                  <c:v>1.0743998712328852E-8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.635633611718462</c:v>
+                  <c:v>2.2029310862081628E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60788954731890454</c:v>
+                  <c:v>6.62582379624653E-10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5817785014060467</c:v>
+                  <c:v>2.5169578386615852E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55718029217017062</c:v>
+                  <c:v>1.11902382227513E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.53398529870481515</c:v>
+                  <c:v>5.5717610463067933E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.51209338675784277</c:v>
+                  <c:v>3.0217544446856245E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.49141295818176528</c:v>
+                  <c:v>1.7519753387167855E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.47186010822715962</c:v>
+                  <c:v>1.071733224747271E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.45335787705616931</c:v>
+                  <c:v>6.8511013022694759E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.43583558374426762</c:v>
+                  <c:v>4.5436512493683723E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1875,49 +1879,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0.66292899807937511</c:v>
+                  <c:v>9.2473169331423033E-9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6344538094827622</c:v>
+                  <c:v>1.9827796622982582E-9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.60762843261091515</c:v>
+                  <c:v>6.1195349877246647E-10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5823333212765216</c:v>
+                  <c:v>2.3639936885783042E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55845927488592828</c:v>
+                  <c:v>1.0634904037017029E-10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.53590640182492966</c:v>
+                  <c:v>5.3417599242697233E-11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.51458320045196215</c:v>
+                  <c:v>2.9166100803685974E-11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.49440574284224464</c:v>
+                  <c:v>1.7000927601757738E-11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.47529694848882231</c:v>
+                  <c:v>1.044535458589108E-11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.45718593691748555</c:v>
+                  <c:v>6.7014085759533707E-12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.44000744966297539</c:v>
+                  <c:v>4.4579307516723526E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:bandFmts/>
-        <c:axId val="140624640"/>
-        <c:axId val="140626560"/>
-        <c:axId val="140640256"/>
+        <c:axId val="206086912"/>
+        <c:axId val="206088832"/>
+        <c:axId val="206082048"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="140624640"/>
+        <c:axId val="206086912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1945,7 +1949,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140626560"/>
+        <c:crossAx val="206088832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1953,7 +1957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140626560"/>
+        <c:axId val="206088832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1964,12 +1968,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140624640"/>
+        <c:crossAx val="206086912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="140640256"/>
+        <c:axId val="206082048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2001,7 +2005,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140626560"/>
+        <c:crossAx val="206088832"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="2"/>
       </c:serAx>
@@ -2357,8 +2361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView tabSelected="1" topLeftCell="O4" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2418,7 +2422,7 @@
         <v>5</v>
       </c>
       <c r="R2" s="2">
-        <v>2.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -2432,54 +2436,54 @@
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <f>($B3+1)^alpha / ($B3+D$2+$C3+1)^beta</f>
-        <v>0.89595845984076194</v>
+        <f>($B3+1)^alpha / ($B3+D$2*$R$4+$C3+1)^beta</f>
+        <v>7.1277811011064909E-3</v>
       </c>
       <c r="E3" s="1">
-        <f>($B3+1)^alpha / ($B3+E$2+$C3+1)^beta</f>
-        <v>0.41205319475393282</v>
+        <f>($B3+1)^alpha / ($B3+E$2*$R$4+$C3+1)^beta</f>
+        <v>1.7736200269505303E-7</v>
       </c>
       <c r="F3" s="1">
-        <f>($B3+1)^alpha / ($B3+F$2+$C3+1)^beta</f>
-        <v>0.22557774482832002</v>
+        <f>($B3+1)^alpha / ($B3+F$2*$R$4+$C3+1)^beta</f>
+        <v>7.552162701187025E-9</v>
       </c>
       <c r="G3" s="1">
-        <f>($B3+1)^alpha / ($B3+G$2+$C3+1)^beta</f>
-        <v>0.13788178155275871</v>
+        <f>($B3+1)^alpha / ($B3+G$2*$R$4+$C3+1)^beta</f>
+        <v>1.1074271680528042E-9</v>
       </c>
       <c r="H3" s="1">
-        <f>($B3+1)^alpha / ($B3+H$2+$C3+1)^beta</f>
-        <v>9.093907957118165E-2</v>
+        <f>($B3+1)^alpha / ($B3+H$2*$R$4+$C3+1)^beta</f>
+        <v>2.775579465207388E-10</v>
       </c>
       <c r="I3" s="1">
-        <f>($B3+1)^alpha / ($B3+I$2+$C3+1)^beta</f>
-        <v>6.3412123590278646E-2</v>
+        <f>($B3+1)^alpha / ($B3+I$2*$R$4+$C3+1)^beta</f>
+        <v>9.4008778546387652E-11</v>
       </c>
       <c r="J3" s="1">
-        <f>($B3+1)^alpha / ($B3+J$2+$C3+1)^beta</f>
-        <v>4.6138182948722822E-2</v>
+        <f>($B3+1)^alpha / ($B3+J$2*$R$4+$C3+1)^beta</f>
+        <v>3.8627071624482668E-11</v>
       </c>
       <c r="K3" s="1">
-        <f>($B3+1)^alpha / ($B3+K$2+$C3+1)^beta</f>
-        <v>3.4714847540041373E-2</v>
+        <f>($B3+1)^alpha / ($B3+K$2*$R$4+$C3+1)^beta</f>
+        <v>1.8157763921595928E-11</v>
       </c>
       <c r="L3" s="1">
-        <f>($B3+1)^alpha / ($B3+L$2+$C3+1)^beta</f>
-        <v>2.6838300568090018E-2</v>
+        <f>($B3+1)^alpha / ($B3+L$2*$R$4+$C3+1)^beta</f>
+        <v>9.4253062960327366E-12</v>
       </c>
       <c r="M3" s="1">
-        <f>($B3+1)^alpha / ($B3+M$2+$C3+1)^beta</f>
-        <v>2.1219048132590373E-2</v>
+        <f>($B3+1)^alpha / ($B3+M$2*$R$4+$C3+1)^beta</f>
+        <v>5.2793486056596163E-12</v>
       </c>
       <c r="N3" s="1">
-        <f>($B3+1)^alpha / ($B3+N$2+$C3+1)^beta</f>
-        <v>1.7094964806248742E-2</v>
+        <f>($B3+1)^alpha / ($B3+N$2*$R$4+$C3+1)^beta</f>
+        <v>3.1407712882628949E-12</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="2">
-        <v>2.7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -2491,51 +2495,58 @@
         <v>4</v>
       </c>
       <c r="C4" s="2">
+        <f>C3</f>
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <f>($B4+1)^alpha / ($B4+D$2+$C4+1)^beta</f>
-        <v>0.85133992252078472</v>
+        <f>($B4+1)^alpha / ($B4+D$2*$R$4+$C4+1)^beta</f>
+        <v>7.1554175279993273E-4</v>
       </c>
       <c r="E4" s="1">
-        <f>($B4+1)^alpha / ($B4+E$2+$C4+1)^beta</f>
-        <v>0.52037165862036061</v>
+        <f>($B4+1)^alpha / ($B4+E$2*$R$4+$C4+1)^beta</f>
+        <v>1.5583542199414839E-7</v>
       </c>
       <c r="F4" s="1">
-        <f>($B4+1)^alpha / ($B4+F$2+$C4+1)^beta</f>
-        <v>0.34320792157561103</v>
+        <f>($B4+1)^alpha / ($B4+F$2*$R$4+$C4+1)^beta</f>
+        <v>7.9159784279003844E-9</v>
       </c>
       <c r="G4" s="1">
-        <f>($B4+1)^alpha / ($B4+G$2+$C4+1)^beta</f>
-        <v>0.23932002877904782</v>
+        <f>($B4+1)^alpha / ($B4+G$2*$R$4+$C4+1)^beta</f>
+        <v>1.2393479666320925E-9</v>
       </c>
       <c r="H4" s="1">
-        <f>($B4+1)^alpha / ($B4+H$2+$C4+1)^beta</f>
-        <v>0.17412744828489032</v>
+        <f>($B4+1)^alpha / ($B4+H$2*$R$4+$C4+1)^beta</f>
+        <v>3.2141804810531992E-10</v>
       </c>
       <c r="I4" s="1">
-        <f>($B4+1)^alpha / ($B4+I$2+$C4+1)^beta</f>
-        <v>0.13101529868361958</v>
+        <f>($B4+1)^alpha / ($B4+I$2*$R$4+$C4+1)^beta</f>
+        <v>1.1117209769583951E-10</v>
       </c>
       <c r="J4" s="1">
-        <f>($B4+1)^alpha / ($B4+J$2+$C4+1)^beta</f>
-        <v>0.10128887822518379</v>
+        <f>($B4+1)^alpha / ($B4+J$2*$R$4+$C4+1)^beta</f>
+        <v>4.6332119348368309E-11</v>
       </c>
       <c r="K4" s="1">
-        <f>($B4+1)^alpha / ($B4+K$2+$C4+1)^beta</f>
-        <v>8.0081582546685598E-2</v>
+        <f>($B4+1)^alpha / ($B4+K$2*$R$4+$C4+1)^beta</f>
+        <v>2.200388571220797E-11</v>
       </c>
       <c r="L4" s="1">
-        <f>($B4+1)^alpha / ($B4+L$2+$C4+1)^beta</f>
-        <v>6.4517118143563507E-2</v>
+        <f>($B4+1)^alpha / ($B4+L$2*$R$4+$C4+1)^beta</f>
+        <v>1.1510445365997865E-11</v>
       </c>
       <c r="M4" s="1">
-        <f>($B4+1)^alpha / ($B4+M$2+$C4+1)^beta</f>
-        <v>5.2817314407941747E-2</v>
+        <f>($B4+1)^alpha / ($B4+M$2*$R$4+$C4+1)^beta</f>
+        <v>6.4864162138221395E-12</v>
       </c>
       <c r="N4" s="1">
-        <f>($B4+1)^alpha / ($B4+N$2+$C4+1)^beta</f>
-        <v>4.3840511427054932E-2</v>
+        <f>($B4+1)^alpha / ($B4+N$2*$R$4+$C4+1)^beta</f>
+        <v>3.8776839725647936E-12</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="R4" s="2">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -2547,51 +2558,52 @@
         <v>6</v>
       </c>
       <c r="C5" s="2">
+        <f t="shared" ref="C5:C32" si="1">C4</f>
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <f>($B5+1)^alpha / ($B5+D$2+$C5+1)^beta</f>
-        <v>0.82317125399304369</v>
+        <f>($B5+1)^alpha / ($B5+D$2*$R$4+$C5+1)^beta</f>
+        <v>1.5741960558485099E-4</v>
       </c>
       <c r="E5" s="1">
-        <f>($B5+1)^alpha / ($B5+E$2+$C5+1)^beta</f>
-        <v>0.57400006180305885</v>
+        <f>($B5+1)^alpha / ($B5+E$2*$R$4+$C5+1)^beta</f>
+        <v>1.2899088739809705E-7</v>
       </c>
       <c r="F5" s="1">
-        <f>($B5+1)^alpha / ($B5+F$2+$C5+1)^beta</f>
-        <v>0.41763811657157218</v>
+        <f>($B5+1)^alpha / ($B5+F$2*$R$4+$C5+1)^beta</f>
+        <v>7.6682831282530988E-9</v>
       </c>
       <c r="G5" s="1">
-        <f>($B5+1)^alpha / ($B5+G$2+$C5+1)^beta</f>
-        <v>0.31423525195617802</v>
+        <f>($B5+1)^alpha / ($B5+G$2*$R$4+$C5+1)^beta</f>
+        <v>1.2762469564477751E-9</v>
       </c>
       <c r="H5" s="1">
-        <f>($B5+1)^alpha / ($B5+H$2+$C5+1)^beta</f>
-        <v>0.2429375537761429</v>
+        <f>($B5+1)^alpha / ($B5+H$2*$R$4+$C5+1)^beta</f>
+        <v>3.419251086247638E-10</v>
       </c>
       <c r="I5" s="1">
-        <f>($B5+1)^alpha / ($B5+I$2+$C5+1)^beta</f>
-        <v>0.1920726550368384</v>
+        <f>($B5+1)^alpha / ($B5+I$2*$R$4+$C5+1)^beta</f>
+        <v>1.2067566792842419E-10</v>
       </c>
       <c r="J5" s="1">
-        <f>($B5+1)^alpha / ($B5+J$2+$C5+1)^beta</f>
-        <v>0.15474187426223007</v>
+        <f>($B5+1)^alpha / ($B5+J$2*$R$4+$C5+1)^beta</f>
+        <v>5.0988826720121202E-11</v>
       </c>
       <c r="K5" s="1">
-        <f>($B5+1)^alpha / ($B5+K$2+$C5+1)^beta</f>
-        <v>0.1266803363224582</v>
+        <f>($B5+1)^alpha / ($B5+K$2*$R$4+$C5+1)^beta</f>
+        <v>2.4457926742693949E-11</v>
       </c>
       <c r="L5" s="1">
-        <f>($B5+1)^alpha / ($B5+L$2+$C5+1)^beta</f>
-        <v>0.10514981298051038</v>
+        <f>($B5+1)^alpha / ($B5+L$2*$R$4+$C5+1)^beta</f>
+        <v>1.2891206680328642E-11</v>
       </c>
       <c r="M5" s="1">
-        <f>($B5+1)^alpha / ($B5+M$2+$C5+1)^beta</f>
-        <v>8.8334621168559044E-2</v>
+        <f>($B5+1)^alpha / ($B5+M$2*$R$4+$C5+1)^beta</f>
+        <v>7.3076832507279356E-12</v>
       </c>
       <c r="N5" s="1">
-        <f>($B5+1)^alpha / ($B5+N$2+$C5+1)^beta</f>
-        <v>7.4996814370496073E-2</v>
+        <f>($B5+1)^alpha / ($B5+N$2*$R$4+$C5+1)^beta</f>
+        <v>4.3895473088157421E-12</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -2603,51 +2615,52 @@
         <v>8</v>
       </c>
       <c r="C6" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D6" s="1">
-        <f>($B6+1)^alpha / ($B6+D$2+$C6+1)^beta</f>
-        <v>0.80274156176023015</v>
+        <f>($B6+1)^alpha / ($B6+D$2*$R$4+$C6+1)^beta</f>
+        <v>5.0805263425290857E-5</v>
       </c>
       <c r="E6" s="1">
-        <f>($B6+1)^alpha / ($B6+E$2+$C6+1)^beta</f>
-        <v>0.60399107961256404</v>
+        <f>($B6+1)^alpha / ($B6+E$2*$R$4+$C6+1)^beta</f>
+        <v>1.0478829777383199E-7</v>
       </c>
       <c r="F6" s="1">
-        <f>($B6+1)^alpha / ($B6+F$2+$C6+1)^beta</f>
-        <v>0.46694988697242207</v>
+        <f>($B6+1)^alpha / ($B6+F$2*$R$4+$C6+1)^beta</f>
+        <v>7.173678459514149E-9</v>
       </c>
       <c r="G6" s="1">
-        <f>($B6+1)^alpha / ($B6+G$2+$C6+1)^beta</f>
-        <v>0.36918254574419912</v>
+        <f>($B6+1)^alpha / ($B6+G$2*$R$4+$C6+1)^beta</f>
+        <v>1.2641975308641976E-9</v>
       </c>
       <c r="H6" s="1">
-        <f>($B6+1)^alpha / ($B6+H$2+$C6+1)^beta</f>
-        <v>0.29742911119962417</v>
+        <f>($B6+1)^alpha / ($B6+H$2*$R$4+$C6+1)^beta</f>
+        <v>3.4935147673396774E-10</v>
       </c>
       <c r="I6" s="1">
-        <f>($B6+1)^alpha / ($B6+I$2+$C6+1)^beta</f>
-        <v>0.24349207361290753</v>
+        <f>($B6+1)^alpha / ($B6+I$2*$R$4+$C6+1)^beta</f>
+        <v>1.2571481127930194E-10</v>
       </c>
       <c r="J6" s="1">
-        <f>($B6+1)^alpha / ($B6+J$2+$C6+1)^beta</f>
-        <v>0.2021082888307339</v>
+        <f>($B6+1)^alpha / ($B6+J$2*$R$4+$C6+1)^beta</f>
+        <v>5.383016257400223E-11</v>
       </c>
       <c r="K6" s="1">
-        <f>($B6+1)^alpha / ($B6+K$2+$C6+1)^beta</f>
-        <v>0.16978783530692243</v>
+        <f>($B6+1)^alpha / ($B6+K$2*$R$4+$C6+1)^beta</f>
+        <v>2.6072533413223757E-11</v>
       </c>
       <c r="L6" s="1">
-        <f>($B6+1)^alpha / ($B6+L$2+$C6+1)^beta</f>
-        <v>0.14415125800543849</v>
+        <f>($B6+1)^alpha / ($B6+L$2*$R$4+$C6+1)^beta</f>
+        <v>1.384403258095006E-11</v>
       </c>
       <c r="M6" s="1">
-        <f>($B6+1)^alpha / ($B6+M$2+$C6+1)^beta</f>
-        <v>0.12353634864011014</v>
+        <f>($B6+1)^alpha / ($B6+M$2*$R$4+$C6+1)^beta</f>
+        <v>7.8934984392986608E-12</v>
       </c>
       <c r="N6" s="1">
-        <f>($B6+1)^alpha / ($B6+N$2+$C6+1)^beta</f>
-        <v>0.10675686255873086</v>
+        <f>($B6+1)^alpha / ($B6+N$2*$R$4+$C6+1)^beta</f>
+        <v>4.7636938529609064E-12</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -2659,51 +2672,52 @@
         <v>10</v>
       </c>
       <c r="C7" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D7" s="1">
-        <f>($B7+1)^alpha / ($B7+D$2+$C7+1)^beta</f>
-        <v>0.7867934421967725</v>
+        <f>($B7+1)^alpha / ($B7+D$2*$R$4+$C7+1)^beta</f>
+        <v>2.0593630529182679E-5</v>
       </c>
       <c r="E7" s="1">
-        <f>($B7+1)^alpha / ($B7+E$2+$C7+1)^beta</f>
-        <v>0.62205905616206081</v>
+        <f>($B7+1)^alpha / ($B7+E$2*$R$4+$C7+1)^beta</f>
+        <v>8.4747450737377282E-8</v>
       </c>
       <c r="F7" s="1">
-        <f>($B7+1)^alpha / ($B7+F$2+$C7+1)^beta</f>
-        <v>0.50115714927691979</v>
+        <f>($B7+1)^alpha / ($B7+F$2*$R$4+$C7+1)^beta</f>
+        <v>6.5899617693384578E-9</v>
       </c>
       <c r="G7" s="1">
-        <f>($B7+1)^alpha / ($B7+G$2+$C7+1)^beta</f>
-        <v>0.41027521815599882</v>
+        <f>($B7+1)^alpha / ($B7+G$2*$R$4+$C7+1)^beta</f>
+        <v>1.2253007990231857E-9</v>
       </c>
       <c r="H7" s="1">
-        <f>($B7+1)^alpha / ($B7+H$2+$C7+1)^beta</f>
-        <v>0.34054505783620453</v>
+        <f>($B7+1)^alpha / ($B7+H$2*$R$4+$C7+1)^beta</f>
+        <v>3.4875494130607935E-10</v>
       </c>
       <c r="I7" s="1">
-        <f>($B7+1)^alpha / ($B7+I$2+$C7+1)^beta</f>
-        <v>0.28608627844503981</v>
+        <f>($B7+1)^alpha / ($B7+I$2*$R$4+$C7+1)^beta</f>
+        <v>1.2787024314771518E-10</v>
       </c>
       <c r="J7" s="1">
-        <f>($B7+1)^alpha / ($B7+J$2+$C7+1)^beta</f>
-        <v>0.2428895854723537</v>
+        <f>($B7+1)^alpha / ($B7+J$2*$R$4+$C7+1)^beta</f>
+        <v>5.5464634477845478E-11</v>
       </c>
       <c r="K7" s="1">
-        <f>($B7+1)^alpha / ($B7+K$2+$C7+1)^beta</f>
-        <v>0.20815421888883184</v>
+        <f>($B7+1)^alpha / ($B7+K$2*$R$4+$C7+1)^beta</f>
+        <v>2.711918423596073E-11</v>
       </c>
       <c r="L7" s="1">
-        <f>($B7+1)^alpha / ($B7+L$2+$C7+1)^beta</f>
-        <v>0.1798813999406158</v>
+        <f>($B7+1)^alpha / ($B7+L$2*$R$4+$C7+1)^beta</f>
+        <v>1.4504017326521389E-11</v>
       </c>
       <c r="M7" s="1">
-        <f>($B7+1)^alpha / ($B7+M$2+$C7+1)^beta</f>
-        <v>0.1566173939180287</v>
+        <f>($B7+1)^alpha / ($B7+M$2*$R$4+$C7+1)^beta</f>
+        <v>8.3169657308462547E-12</v>
       </c>
       <c r="N7" s="1">
-        <f>($B7+1)^alpha / ($B7+N$2+$C7+1)^beta</f>
-        <v>0.13728683268692438</v>
+        <f>($B7+1)^alpha / ($B7+N$2*$R$4+$C7+1)^beta</f>
+        <v>5.0423901194369781E-12</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -2715,51 +2729,52 @@
         <v>12</v>
       </c>
       <c r="C8" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D8" s="1">
-        <f>($B8+1)^alpha / ($B8+D$2+$C8+1)^beta</f>
-        <v>0.773758913061102</v>
+        <f>($B8+1)^alpha / ($B8+D$2*$R$4+$C8+1)^beta</f>
+        <v>9.7107978751659442E-6</v>
       </c>
       <c r="E8" s="1">
-        <f>($B8+1)^alpha / ($B8+E$2+$C8+1)^beta</f>
-        <v>0.63344223925433707</v>
+        <f>($B8+1)^alpha / ($B8+E$2*$R$4+$C8+1)^beta</f>
+        <v>6.8648563583535223E-8</v>
       </c>
       <c r="F8" s="1">
-        <f>($B8+1)^alpha / ($B8+F$2+$C8+1)^beta</f>
-        <v>0.52578272938908455</v>
+        <f>($B8+1)^alpha / ($B8+F$2*$R$4+$C8+1)^beta</f>
+        <v>5.9923531206993966E-9</v>
       </c>
       <c r="G8" s="1">
-        <f>($B8+1)^alpha / ($B8+G$2+$C8+1)^beta</f>
-        <v>0.44170138682190874</v>
+        <f>($B8+1)^alpha / ($B8+G$2*$R$4+$C8+1)^beta</f>
+        <v>1.1717533928321049E-9</v>
       </c>
       <c r="H8" s="1">
-        <f>($B8+1)^alpha / ($B8+H$2+$C8+1)^beta</f>
-        <v>0.37500808263458074</v>
+        <f>($B8+1)^alpha / ($B8+H$2*$R$4+$C8+1)^beta</f>
+        <v>3.4305583235107347E-10</v>
       </c>
       <c r="I8" s="1">
-        <f>($B8+1)^alpha / ($B8+I$2+$C8+1)^beta</f>
-        <v>0.32137859828775811</v>
+        <f>($B8+1)^alpha / ($B8+I$2*$R$4+$C8+1)^beta</f>
+        <v>1.2806961942253445E-10</v>
       </c>
       <c r="J8" s="1">
-        <f>($B8+1)^alpha / ($B8+J$2+$C8+1)^beta</f>
-        <v>0.27772692996354359</v>
+        <f>($B8+1)^alpha / ($B8+J$2*$R$4+$C8+1)^beta</f>
+        <v>5.625118359524747E-11</v>
       </c>
       <c r="K8" s="1">
-        <f>($B8+1)^alpha / ($B8+K$2+$C8+1)^beta</f>
-        <v>0.24180859169488719</v>
+        <f>($B8+1)^alpha / ($B8+K$2*$R$4+$C8+1)^beta</f>
+        <v>2.775807343782481E-11</v>
       </c>
       <c r="L8" s="1">
-        <f>($B8+1)^alpha / ($B8+L$2+$C8+1)^beta</f>
-        <v>0.21196327457505579</v>
+        <f>($B8+1)^alpha / ($B8+L$2*$R$4+$C8+1)^beta</f>
+        <v>1.4950738840146333E-11</v>
       </c>
       <c r="M8" s="1">
-        <f>($B8+1)^alpha / ($B8+M$2+$C8+1)^beta</f>
-        <v>0.18694397710859695</v>
+        <f>($B8+1)^alpha / ($B8+M$2*$R$4+$C8+1)^beta</f>
+        <v>8.6210348293517169E-12</v>
       </c>
       <c r="N8" s="1">
-        <f>($B8+1)^alpha / ($B8+N$2+$C8+1)^beta</f>
-        <v>0.16580115773109833</v>
+        <f>($B8+1)^alpha / ($B8+N$2*$R$4+$C8+1)^beta</f>
+        <v>5.2503961286370369E-12</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -2771,51 +2786,52 @@
         <v>14</v>
       </c>
       <c r="C9" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D9" s="1">
-        <f>($B9+1)^alpha / ($B9+D$2+$C9+1)^beta</f>
-        <v>0.76276520578267581</v>
+        <f>($B9+1)^alpha / ($B9+D$2*$R$4+$C9+1)^beta</f>
+        <v>5.1002249826599734E-6</v>
       </c>
       <c r="E9" s="1">
-        <f>($B9+1)^alpha / ($B9+E$2+$C9+1)^beta</f>
-        <v>0.64078645109772414</v>
+        <f>($B9+1)^alpha / ($B9+E$2*$R$4+$C9+1)^beta</f>
+        <v>5.5851778781637985E-8</v>
       </c>
       <c r="F9" s="1">
-        <f>($B9+1)^alpha / ($B9+F$2+$C9+1)^beta</f>
-        <v>0.54403292716231055</v>
+        <f>($B9+1)^alpha / ($B9+F$2*$R$4+$C9+1)^beta</f>
+        <v>5.417333487789897E-9</v>
       </c>
       <c r="G9" s="1">
-        <f>($B9+1)^alpha / ($B9+G$2+$C9+1)^beta</f>
-        <v>0.46623138980228152</v>
+        <f>($B9+1)^alpha / ($B9+G$2*$R$4+$C9+1)^beta</f>
+        <v>1.1107607757728456E-9</v>
       </c>
       <c r="H9" s="1">
-        <f>($B9+1)^alpha / ($B9+H$2+$C9+1)^beta</f>
-        <v>0.40290490167140708</v>
+        <f>($B9+1)^alpha / ($B9+H$2*$R$4+$C9+1)^beta</f>
+        <v>3.340869456212092E-10</v>
       </c>
       <c r="I9" s="1">
-        <f>($B9+1)^alpha / ($B9+I$2+$C9+1)^beta</f>
-        <v>0.35079733489625498</v>
+        <f>($B9+1)^alpha / ($B9+I$2*$R$4+$C9+1)^beta</f>
+        <v>1.2690991828852465E-10</v>
       </c>
       <c r="J9" s="1">
-        <f>($B9+1)^alpha / ($B9+J$2+$C9+1)^beta</f>
-        <v>0.30750004082003379</v>
+        <f>($B9+1)^alpha / ($B9+J$2*$R$4+$C9+1)^beta</f>
+        <v>5.6423361435155033E-11</v>
       </c>
       <c r="K9" s="1">
-        <f>($B9+1)^alpha / ($B9+K$2+$C9+1)^beta</f>
-        <v>0.27120396543787867</v>
+        <f>($B9+1)^alpha / ($B9+K$2*$R$4+$C9+1)^beta</f>
+        <v>2.8093904802394015E-11</v>
       </c>
       <c r="L9" s="1">
-        <f>($B9+1)^alpha / ($B9+L$2+$C9+1)^beta</f>
-        <v>0.24053158676914244</v>
+        <f>($B9+1)^alpha / ($B9+L$2*$R$4+$C9+1)^beta</f>
+        <v>1.5236274671448739E-11</v>
       </c>
       <c r="M9" s="1">
-        <f>($B9+1)^alpha / ($B9+M$2+$C9+1)^beta</f>
-        <v>0.2144208043939223</v>
+        <f>($B9+1)^alpha / ($B9+M$2*$R$4+$C9+1)^beta</f>
+        <v>8.8338010142549864E-12</v>
       </c>
       <c r="N9" s="1">
-        <f>($B9+1)^alpha / ($B9+N$2+$C9+1)^beta</f>
-        <v>0.1920433398045554</v>
+        <f>($B9+1)^alpha / ($B9+N$2*$R$4+$C9+1)^beta</f>
+        <v>5.4038877366376386E-12</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2827,51 +2843,52 @@
         <v>16</v>
       </c>
       <c r="C10" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D10" s="1">
-        <f>($B10+1)^alpha / ($B10+D$2+$C10+1)^beta</f>
-        <v>0.7532776949250386</v>
+        <f>($B10+1)^alpha / ($B10+D$2*$R$4+$C10+1)^beta</f>
+        <v>2.9038879447843412E-6</v>
       </c>
       <c r="E10" s="1">
-        <f>($B10+1)^alpha / ($B10+E$2+$C10+1)^beta</f>
-        <v>0.6455522985416281</v>
+        <f>($B10+1)^alpha / ($B10+E$2*$R$4+$C10+1)^beta</f>
+        <v>4.5698445331918777E-8</v>
       </c>
       <c r="F10" s="1">
-        <f>($B10+1)^alpha / ($B10+F$2+$C10+1)^beta</f>
-        <v>0.55786931351397562</v>
+        <f>($B10+1)^alpha / ($B10+F$2*$R$4+$C10+1)^beta</f>
+        <v>4.88174719772738E-9</v>
       </c>
       <c r="G10" s="1">
-        <f>($B10+1)^alpha / ($B10+G$2+$C10+1)^beta</f>
-        <v>0.48572024710860967</v>
+        <f>($B10+1)^alpha / ($B10+G$2*$R$4+$C10+1)^beta</f>
+        <v>1.0467283786331982E-9</v>
       </c>
       <c r="H10" s="1">
-        <f>($B10+1)^alpha / ($B10+H$2+$C10+1)^beta</f>
-        <v>0.42577004143200203</v>
+        <f>($B10+1)^alpha / ($B10+H$2*$R$4+$C10+1)^beta</f>
+        <v>3.2305611447847429E-10</v>
       </c>
       <c r="I10" s="1">
-        <f>($B10+1)^alpha / ($B10+I$2+$C10+1)^beta</f>
-        <v>0.37551384804071836</v>
+        <f>($B10+1)^alpha / ($B10+I$2*$R$4+$C10+1)^beta</f>
+        <v>1.2479749151131164E-10</v>
       </c>
       <c r="J10" s="1">
-        <f>($B10+1)^alpha / ($B10+J$2+$C10+1)^beta</f>
-        <v>0.33304432542934098</v>
+        <f>($B10+1)^alpha / ($B10+J$2*$R$4+$C10+1)^beta</f>
+        <v>5.6142677228610724E-11</v>
       </c>
       <c r="K10" s="1">
-        <f>($B10+1)^alpha / ($B10+K$2+$C10+1)^beta</f>
-        <v>0.29689087041166873</v>
+        <f>($B10+1)^alpha / ($B10+K$2*$R$4+$C10+1)^beta</f>
+        <v>2.8199662377501052E-11</v>
       </c>
       <c r="L10" s="1">
-        <f>($B10+1)^alpha / ($B10+L$2+$C10+1)^beta</f>
-        <v>0.26590663379189533</v>
+        <f>($B10+1)^alpha / ($B10+L$2*$R$4+$C10+1)^beta</f>
+        <v>1.5397064023699039E-11</v>
       </c>
       <c r="M10" s="1">
-        <f>($B10+1)^alpha / ($B10+M$2+$C10+1)^beta</f>
-        <v>0.23918787257892171</v>
+        <f>($B10+1)^alpha / ($B10+M$2*$R$4+$C10+1)^beta</f>
+        <v>8.9749525487978353E-12</v>
       </c>
       <c r="N10" s="1">
-        <f>($B10+1)^alpha / ($B10+N$2+$C10+1)^beta</f>
-        <v>0.21601555852892354</v>
+        <f>($B10+1)^alpha / ($B10+N$2*$R$4+$C10+1)^beta</f>
+        <v>5.5142027517397216E-12</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2883,51 +2900,52 @@
         <v>18</v>
       </c>
       <c r="C11" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <f>($B11+1)^alpha / ($B11+D$2+$C11+1)^beta</f>
-        <v>0.7449457381771869</v>
+        <f>($B11+1)^alpha / ($B11+D$2*$R$4+$C11+1)^beta</f>
+        <v>1.7603896062074554E-6</v>
       </c>
       <c r="E11" s="1">
-        <f>($B11+1)^alpha / ($B11+E$2+$C11+1)^beta</f>
-        <v>0.64860213541905876</v>
+        <f>($B11+1)^alpha / ($B11+E$2*$R$4+$C11+1)^beta</f>
+        <v>3.7623354692431818E-8</v>
       </c>
       <c r="F11" s="1">
-        <f>($B11+1)^alpha / ($B11+F$2+$C11+1)^beta</f>
-        <v>0.56854817091556775</v>
+        <f>($B11+1)^alpha / ($B11+F$2*$R$4+$C11+1)^beta</f>
+        <v>4.3921185432816873E-9</v>
       </c>
       <c r="G11" s="1">
-        <f>($B11+1)^alpha / ($B11+G$2+$C11+1)^beta</f>
-        <v>0.50143901797072232</v>
+        <f>($B11+1)^alpha / ($B11+G$2*$R$4+$C11+1)^beta</f>
+        <v>9.823860162910882E-10</v>
       </c>
       <c r="H11" s="1">
-        <f>($B11+1)^alpha / ($B11+H$2+$C11+1)^beta</f>
-        <v>0.44472772536980271</v>
+        <f>($B11+1)^alpha / ($B11+H$2*$R$4+$C11+1)^beta</f>
+        <v>3.1078347045104637E-10</v>
       </c>
       <c r="I11" s="1">
-        <f>($B11+1)^alpha / ($B11+I$2+$C11+1)^beta</f>
-        <v>0.39645053645946332</v>
+        <f>($B11+1)^alpha / ($B11+I$2*$R$4+$C11+1)^beta</f>
+        <v>1.2201922126836812E-10</v>
       </c>
       <c r="J11" s="1">
-        <f>($B11+1)^alpha / ($B11+J$2+$C11+1)^beta</f>
-        <v>0.35507601654693277</v>
+        <f>($B11+1)^alpha / ($B11+J$2*$R$4+$C11+1)^beta</f>
+        <v>5.5525447070035634E-11</v>
       </c>
       <c r="K11" s="1">
-        <f>($B11+1)^alpha / ($B11+K$2+$C11+1)^beta</f>
-        <v>0.31939736060938945</v>
+        <f>($B11+1)^alpha / ($B11+K$2*$R$4+$C11+1)^beta</f>
+        <v>2.81284813169556E-11</v>
       </c>
       <c r="L11" s="1">
-        <f>($B11+1)^alpha / ($B11+L$2+$C11+1)^beta</f>
-        <v>0.28845442078981631</v>
+        <f>($B11+1)^alpha / ($B11+L$2*$R$4+$C11+1)^beta</f>
+        <v>1.5459795458345003E-11</v>
       </c>
       <c r="M11" s="1">
-        <f>($B11+1)^alpha / ($B11+M$2+$C11+1)^beta</f>
-        <v>0.26147650889852803</v>
+        <f>($B11+1)^alpha / ($B11+M$2*$R$4+$C11+1)^beta</f>
+        <v>9.0589556030578899E-12</v>
       </c>
       <c r="N11" s="1">
-        <f>($B11+1)^alpha / ($B11+N$2+$C11+1)^beta</f>
-        <v>0.23783992987563579</v>
+        <f>($B11+1)^alpha / ($B11+N$2*$R$4+$C11+1)^beta</f>
+        <v>5.5896845019651346E-12</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2939,51 +2957,52 @@
         <v>20</v>
       </c>
       <c r="C12" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <f>($B12+1)^alpha / ($B12+D$2+$C12+1)^beta</f>
-        <v>0.73752724891279675</v>
+        <f>($B12+1)^alpha / ($B12+D$2*$R$4+$C12+1)^beta</f>
+        <v>1.1220524896313387E-6</v>
       </c>
       <c r="E12" s="1">
-        <f>($B12+1)^alpha / ($B12+E$2+$C12+1)^beta</f>
-        <v>0.65047248120758128</v>
+        <f>($B12+1)^alpha / ($B12+E$2*$R$4+$C12+1)^beta</f>
+        <v>3.1172193932805887E-8</v>
       </c>
       <c r="F12" s="1">
-        <f>($B12+1)^alpha / ($B12+F$2+$C12+1)^beta</f>
-        <v>0.57690593794196887</v>
+        <f>($B12+1)^alpha / ($B12+F$2*$R$4+$C12+1)^beta</f>
+        <v>3.9495067840919939E-9</v>
       </c>
       <c r="G12" s="1">
-        <f>($B12+1)^alpha / ($B12+G$2+$C12+1)^beta</f>
-        <v>0.5142802113215702</v>
+        <f>($B12+1)^alpha / ($B12+G$2*$R$4+$C12+1)^beta</f>
+        <v>9.194188094111114E-10</v>
       </c>
       <c r="H12" s="1">
-        <f>($B12+1)^alpha / ($B12+H$2+$C12+1)^beta</f>
-        <v>0.46060870658867048</v>
+        <f>($B12+1)^alpha / ($B12+H$2*$R$4+$C12+1)^beta</f>
+        <v>2.9783597742397527E-10</v>
       </c>
       <c r="I12" s="1">
-        <f>($B12+1)^alpha / ($B12+I$2+$C12+1)^beta</f>
-        <v>0.4143259423399569</v>
+        <f>($B12+1)^alpha / ($B12+I$2*$R$4+$C12+1)^beta</f>
+        <v>1.1878269350919362E-10</v>
       </c>
       <c r="J12" s="1">
-        <f>($B12+1)^alpha / ($B12+J$2+$C12+1)^beta</f>
-        <v>0.37418640369426304</v>
+        <f>($B12+1)^alpha / ($B12+J$2*$R$4+$C12+1)^beta</f>
+        <v>5.4657843559496194E-11</v>
       </c>
       <c r="K12" s="1">
-        <f>($B12+1)^alpha / ($B12+K$2+$C12+1)^beta</f>
-        <v>0.33919034503743473</v>
+        <f>($B12+1)^alpha / ($B12+K$2*$R$4+$C12+1)^beta</f>
+        <v>2.7920256509994524E-11</v>
       </c>
       <c r="L12" s="1">
-        <f>($B12+1)^alpha / ($B12+L$2+$C12+1)^beta</f>
-        <v>0.30852870193973403</v>
+        <f>($B12+1)^alpha / ($B12+L$2*$R$4+$C12+1)^beta</f>
+        <v>1.5444665846866091E-11</v>
       </c>
       <c r="M12" s="1">
-        <f>($B12+1)^alpha / ($B12+M$2+$C12+1)^beta</f>
-        <v>0.28154173237033125</v>
+        <f>($B12+1)^alpha / ($B12+M$2*$R$4+$C12+1)^beta</f>
+        <v>9.0968089365131296E-12</v>
       </c>
       <c r="N12" s="1">
-        <f>($B12+1)^alpha / ($B12+N$2+$C12+1)^beta</f>
-        <v>0.25768764288415691</v>
+        <f>($B12+1)^alpha / ($B12+N$2*$R$4+$C12+1)^beta</f>
+        <v>5.636693683808007E-12</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2995,51 +3014,52 @@
         <v>22</v>
       </c>
       <c r="C13" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <f>($B13+1)^alpha / ($B13+D$2+$C13+1)^beta</f>
-        <v>0.73084825842593237</v>
+        <f>($B13+1)^alpha / ($B13+D$2*$R$4+$C13+1)^beta</f>
+        <v>7.4511745618788787E-7</v>
       </c>
       <c r="E13" s="1">
-        <f>($B13+1)^alpha / ($B13+E$2+$C13+1)^beta</f>
-        <v>0.6515114025834452</v>
+        <f>($B13+1)^alpha / ($B13+E$2*$R$4+$C13+1)^beta</f>
+        <v>2.5989704947756442E-8</v>
       </c>
       <c r="F13" s="1">
-        <f>($B13+1)^alpha / ($B13+F$2+$C13+1)^beta</f>
-        <v>0.5835181246825949</v>
+        <f>($B13+1)^alpha / ($B13+F$2*$R$4+$C13+1)^beta</f>
+        <v>3.5521386117832702E-9</v>
       </c>
       <c r="G13" s="1">
-        <f>($B13+1)^alpha / ($B13+G$2+$C13+1)^beta</f>
-        <v>0.52488520825434881</v>
+        <f>($B13+1)^alpha / ($B13+G$2*$R$4+$C13+1)^beta</f>
+        <v>8.5884320665167032E-10</v>
       </c>
       <c r="H13" s="1">
-        <f>($B13+1)^alpha / ($B13+H$2+$C13+1)^beta</f>
-        <v>0.47403478362901474</v>
+        <f>($B13+1)^alpha / ($B13+H$2*$R$4+$C13+1)^beta</f>
+        <v>2.8460925866550344E-10</v>
       </c>
       <c r="I13" s="1">
-        <f>($B13+1)^alpha / ($B13+I$2+$C13+1)^beta</f>
-        <v>0.42970033179037287</v>
+        <f>($B13+1)^alpha / ($B13+I$2*$R$4+$C13+1)^beta</f>
+        <v>1.1524065370859347E-10</v>
       </c>
       <c r="J13" s="1">
-        <f>($B13+1)^alpha / ($B13+J$2+$C13+1)^beta</f>
-        <v>0.39085689651845823</v>
+        <f>($B13+1)^alpha / ($B13+J$2*$R$4+$C13+1)^beta</f>
+        <v>5.3605015652055841E-11</v>
       </c>
       <c r="K13" s="1">
-        <f>($B13+1)^alpha / ($B13+K$2+$C13+1)^beta</f>
-        <v>0.35666868937267632</v>
+        <f>($B13+1)^alpha / ($B13+K$2*$R$4+$C13+1)^beta</f>
+        <v>2.7605625130252493E-11</v>
       </c>
       <c r="L13" s="1">
-        <f>($B13+1)^alpha / ($B13+L$2+$C13+1)^beta</f>
-        <v>0.32644934405011089</v>
+        <f>($B13+1)^alpha / ($B13+L$2*$R$4+$C13+1)^beta</f>
+        <v>1.5367334192817319E-11</v>
       </c>
       <c r="M13" s="1">
-        <f>($B13+1)^alpha / ($B13+M$2+$C13+1)^beta</f>
-        <v>0.29963147499141563</v>
+        <f>($B13+1)^alpha / ($B13+M$2*$R$4+$C13+1)^beta</f>
+        <v>9.0970912203013103E-12</v>
       </c>
       <c r="N13" s="1">
-        <f>($B13+1)^alpha / ($B13+N$2+$C13+1)^beta</f>
-        <v>0.27574315219358198</v>
+        <f>($B13+1)^alpha / ($B13+N$2*$R$4+$C13+1)^beta</f>
+        <v>5.6602100746585705E-12</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -3051,51 +3071,52 @@
         <v>24</v>
       </c>
       <c r="C14" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D14" s="1">
-        <f>($B14+1)^alpha / ($B14+D$2+$C14+1)^beta</f>
-        <v>0.72477966367769564</v>
+        <f>($B14+1)^alpha / ($B14+D$2*$R$4+$C14+1)^beta</f>
+        <v>5.1200000000000003E-7</v>
       </c>
       <c r="E14" s="1">
-        <f>($B14+1)^alpha / ($B14+E$2+$C14+1)^beta</f>
-        <v>0.65195254203100761</v>
+        <f>($B14+1)^alpha / ($B14+E$2*$R$4+$C14+1)^beta</f>
+        <v>2.1801215842470901E-8</v>
       </c>
       <c r="F14" s="1">
-        <f>($B14+1)^alpha / ($B14+F$2+$C14+1)^beta</f>
-        <v>0.58879194410122582</v>
+        <f>($B14+1)^alpha / ($B14+F$2*$R$4+$C14+1)^beta</f>
+        <v>3.1968668679159576E-9</v>
       </c>
       <c r="G14" s="1">
-        <f>($B14+1)^alpha / ($B14+G$2+$C14+1)^beta</f>
-        <v>0.53372474441411333</v>
+        <f>($B14+1)^alpha / ($B14+G$2*$R$4+$C14+1)^beta</f>
+        <v>8.0124077569734154E-10</v>
       </c>
       <c r="H14" s="1">
-        <f>($B14+1)^alpha / ($B14+H$2+$C14+1)^beta</f>
-        <v>0.48547785925047182</v>
+        <f>($B14+1)^alpha / ($B14+H$2*$R$4+$C14+1)^beta</f>
+        <v>2.7137996799972411E-10</v>
       </c>
       <c r="I14" s="1">
-        <f>($B14+1)^alpha / ($B14+I$2+$C14+1)^beta</f>
-        <v>0.44301316753186964</v>
+        <f>($B14+1)^alpha / ($B14+I$2*$R$4+$C14+1)^beta</f>
+        <v>1.1150675100201012E-10</v>
       </c>
       <c r="J14" s="1">
-        <f>($B14+1)^alpha / ($B14+J$2+$C14+1)^beta</f>
-        <v>0.40547814331756116</v>
+        <f>($B14+1)^alpha / ($B14+J$2*$R$4+$C14+1)^beta</f>
+        <v>5.2416949440075422E-11</v>
       </c>
       <c r="K14" s="1">
-        <f>($B14+1)^alpha / ($B14+K$2+$C14+1)^beta</f>
-        <v>0.37216804497659456</v>
+        <f>($B14+1)^alpha / ($B14+K$2*$R$4+$C14+1)^beta</f>
+        <v>2.720851563604588E-11</v>
       </c>
       <c r="L14" s="1">
-        <f>($B14+1)^alpha / ($B14+L$2+$C14+1)^beta</f>
-        <v>0.3424966948833032</v>
+        <f>($B14+1)^alpha / ($B14+L$2*$R$4+$C14+1)^beta</f>
+        <v>1.5240166693117275E-11</v>
       </c>
       <c r="M14" s="1">
-        <f>($B14+1)^alpha / ($B14+M$2+$C14+1)^beta</f>
-        <v>0.31597370786794782</v>
+        <f>($B14+1)^alpha / ($B14+M$2*$R$4+$C14+1)^beta</f>
+        <v>9.0666257437081505E-12</v>
       </c>
       <c r="N14" s="1">
-        <f>($B14+1)^alpha / ($B14+N$2+$C14+1)^beta</f>
-        <v>0.29218660536270025</v>
+        <f>($B14+1)^alpha / ($B14+N$2*$R$4+$C14+1)^beta</f>
+        <v>5.6642130794262971E-12</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -3107,51 +3128,52 @@
         <v>26</v>
       </c>
       <c r="C15" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D15" s="1">
-        <f>($B15+1)^alpha / ($B15+D$2+$C15+1)^beta</f>
-        <v>0.71922309332486423</v>
+        <f>($B15+1)^alpha / ($B15+D$2*$R$4+$C15+1)^beta</f>
+        <v>3.6212879647952505E-7</v>
       </c>
       <c r="E15" s="1">
-        <f>($B15+1)^alpha / ($B15+E$2+$C15+1)^beta</f>
-        <v>0.65195722446152593</v>
+        <f>($B15+1)^alpha / ($B15+E$2*$R$4+$C15+1)^beta</f>
+        <v>1.8395071572117217E-8</v>
       </c>
       <c r="F15" s="1">
-        <f>($B15+1)^alpha / ($B15+F$2+$C15+1)^beta</f>
-        <v>0.59302252887282747</v>
+        <f>($B15+1)^alpha / ($B15+F$2*$R$4+$C15+1)^beta</f>
+        <v>2.8799844209532715E-9</v>
       </c>
       <c r="G15" s="1">
-        <f>($B15+1)^alpha / ($B15+G$2+$C15+1)^beta</f>
-        <v>0.54115091744723187</v>
+        <f>($B15+1)^alpha / ($B15+G$2*$R$4+$C15+1)^beta</f>
+        <v>7.4690804848943912E-10</v>
       </c>
       <c r="H15" s="1">
-        <f>($B15+1)^alpha / ($B15+H$2+$C15+1)^beta</f>
-        <v>0.49530100986290276</v>
+        <f>($B15+1)^alpha / ($B15+H$2*$R$4+$C15+1)^beta</f>
+        <v>2.5834060976335819E-10</v>
       </c>
       <c r="I15" s="1">
-        <f>($B15+1)^alpha / ($B15+I$2+$C15+1)^beta</f>
-        <v>0.45461194777949454</v>
+        <f>($B15+1)^alpha / ($B15+I$2*$R$4+$C15+1)^beta</f>
+        <v>1.0766611597843494E-10</v>
       </c>
       <c r="J15" s="1">
-        <f>($B15+1)^alpha / ($B15+J$2+$C15+1)^beta</f>
-        <v>0.41836770155462916</v>
+        <f>($B15+1)^alpha / ($B15+J$2*$R$4+$C15+1)^beta</f>
+        <v>5.1132409749139679E-11</v>
       </c>
       <c r="K15" s="1">
-        <f>($B15+1)^alpha / ($B15+K$2+$C15+1)^beta</f>
-        <v>0.38596925426520845</v>
+        <f>($B15+1)^alpha / ($B15+K$2*$R$4+$C15+1)^beta</f>
+        <v>2.6747857925964039E-11</v>
       </c>
       <c r="L15" s="1">
-        <f>($B15+1)^alpha / ($B15+L$2+$C15+1)^beta</f>
-        <v>0.35691275371954456</v>
+        <f>($B15+1)^alpha / ($B15+L$2*$R$4+$C15+1)^beta</f>
+        <v>1.507306918362175E-11</v>
       </c>
       <c r="M15" s="1">
-        <f>($B15+1)^alpha / ($B15+M$2+$C15+1)^beta</f>
-        <v>0.33077222508506426</v>
+        <f>($B15+1)^alpha / ($B15+M$2*$R$4+$C15+1)^beta</f>
+        <v>9.0109232685593169E-12</v>
       </c>
       <c r="N15" s="1">
-        <f>($B15+1)^alpha / ($B15+N$2+$C15+1)^beta</f>
-        <v>0.30718579699177939</v>
+        <f>($B15+1)^alpha / ($B15+N$2*$R$4+$C15+1)^beta</f>
+        <v>5.651934442654422E-12</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -3163,51 +3185,52 @@
         <v>28</v>
       </c>
       <c r="C16" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D16" s="1">
-        <f>($B16+1)^alpha / ($B16+D$2+$C16+1)^beta</f>
-        <v>0.71410191909521781</v>
+        <f>($B16+1)^alpha / ($B16+D$2*$R$4+$C16+1)^beta</f>
+        <v>2.6254817841431038E-7</v>
       </c>
       <c r="E16" s="1">
-        <f>($B16+1)^alpha / ($B16+E$2+$C16+1)^beta</f>
-        <v>0.65163950753054223</v>
+        <f>($B16+1)^alpha / ($B16+E$2*$R$4+$C16+1)^beta</f>
+        <v>1.5608030981867192E-8</v>
       </c>
       <c r="F16" s="1">
-        <f>($B16+1)^alpha / ($B16+F$2+$C16+1)^beta</f>
-        <v>0.59642827119093744</v>
+        <f>($B16+1)^alpha / ($B16+F$2*$R$4+$C16+1)^beta</f>
+        <v>2.5976743038292667E-9</v>
       </c>
       <c r="G16" s="1">
-        <f>($B16+1)^alpha / ($B16+G$2+$C16+1)^beta</f>
-        <v>0.54743158741372244</v>
+        <f>($B16+1)^alpha / ($B16+G$2*$R$4+$C16+1)^beta</f>
+        <v>6.9595470063314969E-10</v>
       </c>
       <c r="H16" s="1">
-        <f>($B16+1)^alpha / ($B16+H$2+$C16+1)^beta</f>
-        <v>0.50378723239312873</v>
+        <f>($B16+1)^alpha / ($B16+H$2*$R$4+$C16+1)^beta</f>
+        <v>2.4562337257015717E-10</v>
       </c>
       <c r="I16" s="1">
-        <f>($B16+1)^alpha / ($B16+I$2+$C16+1)^beta</f>
-        <v>0.46477388592034746</v>
+        <f>($B16+1)^alpha / ($B16+I$2*$R$4+$C16+1)^beta</f>
+        <v>1.037827077934207E-10</v>
       </c>
       <c r="J16" s="1">
-        <f>($B16+1)^alpha / ($B16+J$2+$C16+1)^beta</f>
-        <v>0.42978482261901124</v>
+        <f>($B16+1)^alpha / ($B16+J$2*$R$4+$C16+1)^beta</f>
+        <v>4.9781688021627458E-11</v>
       </c>
       <c r="K16" s="1">
-        <f>($B16+1)^alpha / ($B16+K$2+$C16+1)^beta</f>
-        <v>0.39830709495236305</v>
+        <f>($B16+1)^alpha / ($B16+K$2*$R$4+$C16+1)^beta</f>
+        <v>2.6238774689851504E-11</v>
       </c>
       <c r="L16" s="1">
-        <f>($B16+1)^alpha / ($B16+L$2+$C16+1)^beta</f>
-        <v>0.36990494706427146</v>
+        <f>($B16+1)^alpha / ($B16+L$2*$R$4+$C16+1)^beta</f>
+        <v>1.487406563834284E-11</v>
       </c>
       <c r="M16" s="1">
-        <f>($B16+1)^alpha / ($B16+M$2+$C16+1)^beta</f>
-        <v>0.34420651298245203</v>
+        <f>($B16+1)^alpha / ($B16+M$2*$R$4+$C16+1)^beta</f>
+        <v>8.9344888870809753E-12</v>
       </c>
       <c r="N16" s="1">
-        <f>($B16+1)^alpha / ($B16+N$2+$C16+1)^beta</f>
-        <v>0.32089308284436174</v>
+        <f>($B16+1)^alpha / ($B16+N$2*$R$4+$C16+1)^beta</f>
+        <v>5.6260328476689453E-12</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -3219,51 +3242,52 @@
         <v>30</v>
       </c>
       <c r="C17" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D17" s="1">
-        <f>($B17+1)^alpha / ($B17+D$2+$C17+1)^beta</f>
-        <v>0.70935532069514695</v>
+        <f>($B17+1)^alpha / ($B17+D$2*$R$4+$C17+1)^beta</f>
+        <v>1.9447884999558742E-7</v>
       </c>
       <c r="E17" s="1">
-        <f>($B17+1)^alpha / ($B17+E$2+$C17+1)^beta</f>
-        <v>0.65108166062134665</v>
+        <f>($B17+1)^alpha / ($B17+E$2*$R$4+$C17+1)^beta</f>
+        <v>1.3313783759094749E-8</v>
       </c>
       <c r="F17" s="1">
-        <f>($B17+1)^alpha / ($B17+F$2+$C17+1)^beta</f>
-        <v>0.59917373313436306</v>
+        <f>($B17+1)^alpha / ($B17+F$2*$R$4+$C17+1)^beta</f>
+        <v>2.3462513199744615E-9</v>
       </c>
       <c r="G17" s="1">
-        <f>($B17+1)^alpha / ($B17+G$2+$C17+1)^beta</f>
-        <v>0.55277364407867324</v>
+        <f>($B17+1)^alpha / ($B17+G$2*$R$4+$C17+1)^beta</f>
+        <v>6.4836890075380893E-10</v>
       </c>
       <c r="H17" s="1">
-        <f>($B17+1)^alpha / ($B17+H$2+$C17+1)^beta</f>
-        <v>0.51115979138624024</v>
+        <f>($B17+1)^alpha / ($B17+H$2*$R$4+$C17+1)^beta</f>
+        <v>2.3331681537359964E-10</v>
       </c>
       <c r="I17" s="1">
-        <f>($B17+1)^alpha / ($B17+I$2+$C17+1)^beta</f>
-        <v>0.47372210661797171</v>
+        <f>($B17+1)^alpha / ($B17+I$2*$R$4+$C17+1)^beta</f>
+        <v>9.9904553608291998E-11</v>
       </c>
       <c r="J17" s="1">
-        <f>($B17+1)^alpha / ($B17+J$2+$C17+1)^beta</f>
-        <v>0.43994232840028497</v>
+        <f>($B17+1)^alpha / ($B17+J$2*$R$4+$C17+1)^beta</f>
+        <v>4.8388574128947406E-11</v>
       </c>
       <c r="K17" s="1">
-        <f>($B17+1)^alpha / ($B17+K$2+$C17+1)^beta</f>
-        <v>0.40937818208127802</v>
+        <f>($B17+1)^alpha / ($B17+K$2*$R$4+$C17+1)^beta</f>
+        <v>2.569343708069049E-11</v>
       </c>
       <c r="L17" s="1">
-        <f>($B17+1)^alpha / ($B17+L$2+$C17+1)^beta</f>
-        <v>0.38165061363606145</v>
+        <f>($B17+1)^alpha / ($B17+L$2*$R$4+$C17+1)^beta</f>
+        <v>1.4649713102793827E-11</v>
       </c>
       <c r="M17" s="1">
-        <f>($B17+1)^alpha / ($B17+M$2+$C17+1)^beta</f>
-        <v>0.35643342794550431</v>
+        <f>($B17+1)^alpha / ($B17+M$2*$R$4+$C17+1)^beta</f>
+        <v>8.8410416233160572E-12</v>
       </c>
       <c r="N17" s="1">
-        <f>($B17+1)^alpha / ($B17+N$2+$C17+1)^beta</f>
-        <v>0.33344483205307562</v>
+        <f>($B17+1)^alpha / ($B17+N$2*$R$4+$C17+1)^beta</f>
+        <v>5.5887185574799863E-12</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -3275,51 +3299,52 @@
         <v>32</v>
       </c>
       <c r="C18" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D18" s="1">
-        <f>($B18+1)^alpha / ($B18+D$2+$C18+1)^beta</f>
-        <v>0.70493424068343191</v>
+        <f>($B18+1)^alpha / ($B18+D$2*$R$4+$C18+1)^beta</f>
+        <v>1.4678689048907796E-7</v>
       </c>
       <c r="E18" s="1">
-        <f>($B18+1)^alpha / ($B18+E$2+$C18+1)^beta</f>
-        <v>0.65034404465629492</v>
+        <f>($B18+1)^alpha / ($B18+E$2*$R$4+$C18+1)^beta</f>
+        <v>1.1414148604430704E-8</v>
       </c>
       <c r="F18" s="1">
-        <f>($B18+1)^alpha / ($B18+F$2+$C18+1)^beta</f>
-        <v>0.601384906384</v>
+        <f>($B18+1)^alpha / ($B18+F$2*$R$4+$C18+1)^beta</f>
+        <v>2.1222832384628993E-9</v>
       </c>
       <c r="G18" s="1">
-        <f>($B18+1)^alpha / ($B18+G$2+$C18+1)^beta</f>
-        <v>0.55733907388895809</v>
+        <f>($B18+1)^alpha / ($B18+G$2*$R$4+$C18+1)^beta</f>
+        <v>6.0406127773283111E-10</v>
       </c>
       <c r="H18" s="1">
-        <f>($B18+1)^alpha / ($B18+H$2+$C18+1)^beta</f>
-        <v>0.51759680717814449</v>
+        <f>($B18+1)^alpha / ($B18+H$2*$R$4+$C18+1)^beta</f>
+        <v>2.2147775790802882E-10</v>
       </c>
       <c r="I18" s="1">
-        <f>($B18+1)^alpha / ($B18+I$2+$C18+1)^beta</f>
-        <v>0.48163776544108811</v>
+        <f>($B18+1)^alpha / ($B18+I$2*$R$4+$C18+1)^beta</f>
+        <v>9.6067564938864846E-11</v>
       </c>
       <c r="J18" s="1">
-        <f>($B18+1)^alpha / ($B18+J$2+$C18+1)^beta</f>
-        <v>0.44901598760433586</v>
+        <f>($B18+1)^alpha / ($B18+J$2*$R$4+$C18+1)^beta</f>
+        <v>4.6971804956504952E-11</v>
       </c>
       <c r="K18" s="1">
-        <f>($B18+1)^alpha / ($B18+K$2+$C18+1)^beta</f>
-        <v>0.4193477016566946</v>
+        <f>($B18+1)^alpha / ($B18+K$2*$R$4+$C18+1)^beta</f>
+        <v>2.512169492339436E-11</v>
       </c>
       <c r="L18" s="1">
-        <f>($B18+1)^alpha / ($B18+L$2+$C18+1)^beta</f>
-        <v>0.39230137520137004</v>
+        <f>($B18+1)^alpha / ($B18+L$2*$R$4+$C18+1)^beta</f>
+        <v>1.4405407210634934E-11</v>
       </c>
       <c r="M18" s="1">
-        <f>($B18+1)^alpha / ($B18+M$2+$C18+1)^beta</f>
-        <v>0.36758955256988063</v>
+        <f>($B18+1)^alpha / ($B18+M$2*$R$4+$C18+1)^beta</f>
+        <v>8.7336758784481444E-12</v>
       </c>
       <c r="N18" s="1">
-        <f>($B18+1)^alpha / ($B18+N$2+$C18+1)^beta</f>
-        <v>0.34496212431913259</v>
+        <f>($B18+1)^alpha / ($B18+N$2*$R$4+$C18+1)^beta</f>
+        <v>5.5418448626566281E-12</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -3331,51 +3356,52 @@
         <v>34</v>
       </c>
       <c r="C19" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D19" s="1">
-        <f>($B19+1)^alpha / ($B19+D$2+$C19+1)^beta</f>
-        <v>0.70079855159577498</v>
+        <f>($B19+1)^alpha / ($B19+D$2*$R$4+$C19+1)^beta</f>
+        <v>1.1264030050525835E-7</v>
       </c>
       <c r="E19" s="1">
-        <f>($B19+1)^alpha / ($B19+E$2+$C19+1)^beta</f>
-        <v>0.64947159727968862</v>
+        <f>($B19+1)^alpha / ($B19+E$2*$R$4+$C19+1)^beta</f>
+        <v>9.8324046566225758E-9</v>
       </c>
       <c r="F19" s="1">
-        <f>($B19+1)^alpha / ($B19+F$2+$C19+1)^beta</f>
-        <v>0.60315962195005268</v>
+        <f>($B19+1)^alpha / ($B19+F$2*$R$4+$C19+1)^beta</f>
+        <v>1.9226426220274217E-9</v>
       </c>
       <c r="G19" s="1">
-        <f>($B19+1)^alpha / ($B19+G$2+$C19+1)^beta</f>
-        <v>0.5612562683763429</v>
+        <f>($B19+1)^alpha / ($B19+G$2*$R$4+$C19+1)^beta</f>
+        <v>5.6289469187632616E-10</v>
       </c>
       <c r="H19" s="1">
-        <f>($B19+1)^alpha / ($B19+H$2+$C19+1)^beta</f>
-        <v>0.52324185461937778</v>
+        <f>($B19+1)^alpha / ($B19+H$2*$R$4+$C19+1)^beta</f>
+        <v>2.1013987277088866E-10</v>
       </c>
       <c r="I19" s="1">
-        <f>($B19+1)^alpha / ($B19+I$2+$C19+1)^beta</f>
-        <v>0.48866916814234079</v>
+        <f>($B19+1)^alpha / ($B19+I$2*$R$4+$C19+1)^beta</f>
+        <v>9.22983656640531E-11</v>
       </c>
       <c r="J19" s="1">
-        <f>($B19+1)^alpha / ($B19+J$2+$C19+1)^beta</f>
-        <v>0.45715187164109583</v>
+        <f>($B19+1)^alpha / ($B19+J$2*$R$4+$C19+1)^beta</f>
+        <v>4.5546149406009183E-11</v>
       </c>
       <c r="K19" s="1">
-        <f>($B19+1)^alpha / ($B19+K$2+$C19+1)^beta</f>
-        <v>0.42835499076896194</v>
+        <f>($B19+1)^alpha / ($B19+K$2*$R$4+$C19+1)^beta</f>
+        <v>2.4531550666467651E-11</v>
       </c>
       <c r="L19" s="1">
-        <f>($B19+1)^alpha / ($B19+L$2+$C19+1)^beta</f>
-        <v>0.40198707102882753</v>
+        <f>($B19+1)^alpha / ($B19+L$2*$R$4+$C19+1)^beta</f>
+        <v>1.4145612131604462E-11</v>
       </c>
       <c r="M19" s="1">
-        <f>($B19+1)^alpha / ($B19+M$2+$C19+1)^beta</f>
-        <v>0.37779368029300103</v>
+        <f>($B19+1)^alpha / ($B19+M$2*$R$4+$C19+1)^beta</f>
+        <v>8.6149828463878401E-12</v>
       </c>
       <c r="N19" s="1">
-        <f>($B19+1)^alpha / ($B19+N$2+$C19+1)^beta</f>
-        <v>0.355552001803769</v>
+        <f>($B19+1)^alpha / ($B19+N$2*$R$4+$C19+1)^beta</f>
+        <v>5.4869767505563733E-12</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -3387,51 +3413,52 @@
         <v>36</v>
       </c>
       <c r="C20" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D20" s="1">
-        <f>($B20+1)^alpha / ($B20+D$2+$C20+1)^beta</f>
-        <v>0.69691502481948309</v>
+        <f>($B20+1)^alpha / ($B20+D$2*$R$4+$C20+1)^beta</f>
+        <v>8.7718711095448732E-8</v>
       </c>
       <c r="E20" s="1">
-        <f>($B20+1)^alpha / ($B20+E$2+$C20+1)^beta</f>
-        <v>0.64849819512284956</v>
+        <f>($B20+1)^alpha / ($B20+E$2*$R$4+$C20+1)^beta</f>
+        <v>8.5082609988308973E-9</v>
       </c>
       <c r="F20" s="1">
-        <f>($B20+1)^alpha / ($B20+F$2+$C20+1)^beta</f>
-        <v>0.60457480379688433</v>
+        <f>($B20+1)^alpha / ($B20+F$2*$R$4+$C20+1)^beta</f>
+        <v>1.7445192563537052E-9</v>
       </c>
       <c r="G20" s="1">
-        <f>($B20+1)^alpha / ($B20+G$2+$C20+1)^beta</f>
-        <v>0.5646281233869419</v>
+        <f>($B20+1)^alpha / ($B20+G$2*$R$4+$C20+1)^beta</f>
+        <v>5.2470443919580889E-10</v>
       </c>
       <c r="H20" s="1">
-        <f>($B20+1)^alpha / ($B20+H$2+$C20+1)^beta</f>
-        <v>0.52821176414460025</v>
+        <f>($B20+1)^alpha / ($B20+H$2*$R$4+$C20+1)^beta</f>
+        <v>1.9931996259281205E-10</v>
       </c>
       <c r="I20" s="1">
-        <f>($B20+1)^alpha / ($B20+I$2+$C20+1)^beta</f>
-        <v>0.4949386831600962</v>
+        <f>($B20+1)^alpha / ($B20+I$2*$R$4+$C20+1)^beta</f>
+        <v>8.8616417394957229E-11</v>
       </c>
       <c r="J20" s="1">
-        <f>($B20+1)^alpha / ($B20+J$2+$C20+1)^beta</f>
-        <v>0.46447212211822392</v>
+        <f>($B20+1)^alpha / ($B20+J$2*$R$4+$C20+1)^beta</f>
+        <v>4.4123234257928975E-11</v>
       </c>
       <c r="K20" s="1">
-        <f>($B20+1)^alpha / ($B20+K$2+$C20+1)^beta</f>
-        <v>0.43651809984694823</v>
+        <f>($B20+1)^alpha / ($B20+K$2*$R$4+$C20+1)^beta</f>
+        <v>2.3929522124998264E-11</v>
       </c>
       <c r="L20" s="1">
-        <f>($B20+1)^alpha / ($B20+L$2+$C20+1)^beta</f>
-        <v>0.41081916485153885</v>
+        <f>($B20+1)^alpha / ($B20+L$2*$R$4+$C20+1)^beta</f>
+        <v>1.3874036887413698E-11</v>
       </c>
       <c r="M20" s="1">
-        <f>($B20+1)^alpha / ($B20+M$2+$C20+1)^beta</f>
-        <v>0.38714917401783949</v>
+        <f>($B20+1)^alpha / ($B20+M$2*$R$4+$C20+1)^beta</f>
+        <v>8.4871436058576603E-12</v>
       </c>
       <c r="N20" s="1">
-        <f>($B20+1)^alpha / ($B20+N$2+$C20+1)^beta</f>
-        <v>0.3653089110318512</v>
+        <f>($B20+1)^alpha / ($B20+N$2*$R$4+$C20+1)^beta</f>
+        <v>5.4254435029156751E-12</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -3443,51 +3470,52 @@
         <v>38</v>
       </c>
       <c r="C21" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D21" s="1">
-        <f>($B21+1)^alpha / ($B21+D$2+$C21+1)^beta</f>
-        <v>0.69325584403428708</v>
+        <f>($B21+1)^alpha / ($B21+D$2*$R$4+$C21+1)^beta</f>
+        <v>6.9216441571272889E-8</v>
       </c>
       <c r="E21" s="1">
-        <f>($B21+1)^alpha / ($B21+E$2+$C21+1)^beta</f>
-        <v>0.64744965186411763</v>
+        <f>($B21+1)^alpha / ($B21+E$2*$R$4+$C21+1)^beta</f>
+        <v>7.3940626912577473E-9</v>
       </c>
       <c r="F21" s="1">
-        <f>($B21+1)^alpha / ($B21+F$2+$C21+1)^beta</f>
-        <v>0.6056916200959146</v>
+        <f>($B21+1)^alpha / ($B21+F$2*$R$4+$C21+1)^beta</f>
+        <v>1.5854109069669731E-9</v>
       </c>
       <c r="G21" s="1">
-        <f>($B21+1)^alpha / ($B21+G$2+$C21+1)^beta</f>
-        <v>0.56753793308039824</v>
+        <f>($B21+1)^alpha / ($B21+G$2*$R$4+$C21+1)^beta</f>
+        <v>4.8931193412882969E-10</v>
       </c>
       <c r="H21" s="1">
-        <f>($B21+1)^alpha / ($B21+H$2+$C21+1)^beta</f>
-        <v>0.53260243567418941</v>
+        <f>($B21+1)^alpha / ($B21+H$2*$R$4+$C21+1)^beta</f>
+        <v>1.8902258526945462E-10</v>
       </c>
       <c r="I21" s="1">
-        <f>($B21+1)^alpha / ($B21+I$2+$C21+1)^beta</f>
-        <v>0.5005480245705185</v>
+        <f>($B21+1)^alpha / ($B21+I$2*$R$4+$C21+1)^beta</f>
+        <v>8.5035635453767495E-11</v>
       </c>
       <c r="J21" s="1">
-        <f>($B21+1)^alpha / ($B21+J$2+$C21+1)^beta</f>
-        <v>0.47107948443431674</v>
+        <f>($B21+1)^alpha / ($B21+J$2*$R$4+$C21+1)^beta</f>
+        <v>4.2712181324877666E-11</v>
       </c>
       <c r="K21" s="1">
-        <f>($B21+1)^alpha / ($B21+K$2+$C21+1)^beta</f>
-        <v>0.44393750072833837</v>
+        <f>($B21+1)^alpha / ($B21+K$2*$R$4+$C21+1)^beta</f>
+        <v>2.3320924259564187E-11</v>
       </c>
       <c r="L21" s="1">
-        <f>($B21+1)^alpha / ($B21+L$2+$C21+1)^beta</f>
-        <v>0.41889363542797609</v>
+        <f>($B21+1)^alpha / ($B21+L$2*$R$4+$C21+1)^beta</f>
+        <v>1.3593772702480002E-11</v>
       </c>
       <c r="M21" s="1">
-        <f>($B21+1)^alpha / ($B21+M$2+$C21+1)^beta</f>
-        <v>0.39574609424648566</v>
+        <f>($B21+1)^alpha / ($B21+M$2*$R$4+$C21+1)^beta</f>
+        <v>8.3520016885860879E-12</v>
       </c>
       <c r="N21" s="1">
-        <f>($B21+1)^alpha / ($B21+N$2+$C21+1)^beta</f>
-        <v>0.37431614731721402</v>
+        <f>($B21+1)^alpha / ($B21+N$2*$R$4+$C21+1)^beta</f>
+        <v>5.3583796779736705E-12</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -3499,51 +3527,52 @@
         <v>40</v>
       </c>
       <c r="C22" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D22" s="1">
-        <f>($B22+1)^alpha / ($B22+D$2+$C22+1)^beta</f>
-        <v>0.68979749727836415</v>
+        <f>($B22+1)^alpha / ($B22+D$2*$R$4+$C22+1)^beta</f>
+        <v>5.5267859485853923E-8</v>
       </c>
       <c r="E22" s="1">
-        <f>($B22+1)^alpha / ($B22+E$2+$C22+1)^beta</f>
-        <v>0.64634581833475013</v>
+        <f>($B22+1)^alpha / ($B22+E$2*$R$4+$C22+1)^beta</f>
+        <v>6.45192308021738E-9</v>
       </c>
       <c r="F22" s="1">
-        <f>($B22+1)^alpha / ($B22+F$2+$C22+1)^beta</f>
-        <v>0.60655920435920663</v>
+        <f>($B22+1)^alpha / ($B22+F$2*$R$4+$C22+1)^beta</f>
+        <v>1.4431029011925225E-9</v>
       </c>
       <c r="G22" s="1">
-        <f>($B22+1)^alpha / ($B22+G$2+$C22+1)^beta</f>
-        <v>0.57005374213646276</v>
+        <f>($B22+1)^alpha / ($B22+G$2*$R$4+$C22+1)^beta</f>
+        <v>4.5653390868065248E-10</v>
       </c>
       <c r="H22" s="1">
-        <f>($B22+1)^alpha / ($B22+H$2+$C22+1)^beta</f>
-        <v>0.53649322295480373</v>
+        <f>($B22+1)^alpha / ($B22+H$2*$R$4+$C22+1)^beta</f>
+        <v>1.7924348402111083E-10</v>
       </c>
       <c r="I22" s="1">
-        <f>($B22+1)^alpha / ($B22+I$2+$C22+1)^beta</f>
-        <v>0.5055823240577888</v>
+        <f>($B22+1)^alpha / ($B22+I$2*$R$4+$C22+1)^beta</f>
+        <v>8.1565629424673608E-11</v>
       </c>
       <c r="J22" s="1">
-        <f>($B22+1)^alpha / ($B22+J$2+$C22+1)^beta</f>
-        <v>0.47706088669065017</v>
+        <f>($B22+1)^alpha / ($B22+J$2*$R$4+$C22+1)^beta</f>
+        <v>4.1320104644700577E-11</v>
       </c>
       <c r="K22" s="1">
-        <f>($B22+1)^alpha / ($B22+K$2+$C22+1)^beta</f>
-        <v>0.45069909556563592</v>
+        <f>($B22+1)^alpha / ($B22+K$2*$R$4+$C22+1)^beta</f>
+        <v>2.2710090848005329E-11</v>
       </c>
       <c r="L22" s="1">
-        <f>($B22+1)^alpha / ($B22+L$2+$C22+1)^beta</f>
-        <v>0.42629340252289766</v>
+        <f>($B22+1)^alpha / ($B22+L$2*$R$4+$C22+1)^beta</f>
+        <v>1.3307401465162417E-11</v>
       </c>
       <c r="M22" s="1">
-        <f>($B22+1)^alpha / ($B22+M$2+$C22+1)^beta</f>
-        <v>0.40366306713552463</v>
+        <f>($B22+1)^alpha / ($B22+M$2*$R$4+$C22+1)^beta</f>
+        <v>8.2111204636147892E-12</v>
       </c>
       <c r="N22" s="1">
-        <f>($B22+1)^alpha / ($B22+N$2+$C22+1)^beta</f>
-        <v>0.38264721079844616</v>
+        <f>($B22+1)^alpha / ($B22+N$2*$R$4+$C22+1)^beta</f>
+        <v>5.2867575194940816E-12</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -3555,51 +3584,52 @@
         <v>42</v>
       </c>
       <c r="C23" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D23" s="1">
-        <f>($B23+1)^alpha / ($B23+D$2+$C23+1)^beta</f>
-        <v>0.68651993776308051</v>
+        <f>($B23+1)^alpha / ($B23+D$2*$R$4+$C23+1)^beta</f>
+        <v>4.4605863380935203E-8</v>
       </c>
       <c r="E23" s="1">
-        <f>($B23+1)^alpha / ($B23+E$2+$C23+1)^beta</f>
-        <v>0.64520207880874014</v>
+        <f>($B23+1)^alpha / ($B23+E$2*$R$4+$C23+1)^beta</f>
+        <v>5.6515483129944283E-9</v>
       </c>
       <c r="F23" s="1">
-        <f>($B23+1)^alpha / ($B23+F$2+$C23+1)^beta</f>
-        <v>0.60721738518888235</v>
+        <f>($B23+1)^alpha / ($B23+F$2*$R$4+$C23+1)^beta</f>
+        <v>1.3156427132096505E-9</v>
       </c>
       <c r="G23" s="1">
-        <f>($B23+1)^alpha / ($B23+G$2+$C23+1)^beta</f>
-        <v>0.57223160270554141</v>
+        <f>($B23+1)^alpha / ($B23+G$2*$R$4+$C23+1)^beta</f>
+        <v>4.2618851106657757E-10</v>
       </c>
       <c r="H23" s="1">
-        <f>($B23+1)^alpha / ($B23+H$2+$C23+1)^beta</f>
-        <v>0.53995027671876117</v>
+        <f>($B23+1)^alpha / ($B23+H$2*$R$4+$C23+1)^beta</f>
+        <v>1.6997214280495356E-10</v>
       </c>
       <c r="I23" s="1">
-        <f>($B23+1)^alpha / ($B23+I$2+$C23+1)^beta</f>
-        <v>0.51011329613648237</v>
+        <f>($B23+1)^alpha / ($B23+I$2*$R$4+$C23+1)^beta</f>
+        <v>7.82126631114527E-11</v>
       </c>
       <c r="J23" s="1">
-        <f>($B23+1)^alpha / ($B23+J$2+$C23+1)^beta</f>
-        <v>0.48249027970486097</v>
+        <f>($B23+1)^alpha / ($B23+J$2*$R$4+$C23+1)^beta</f>
+        <v>3.9952502224580523E-11</v>
       </c>
       <c r="K23" s="1">
-        <f>($B23+1)^alpha / ($B23+K$2+$C23+1)^beta</f>
-        <v>0.45687666057247966</v>
+        <f>($B23+1)^alpha / ($B23+K$2*$R$4+$C23+1)^beta</f>
+        <v>2.2100550773376159E-11</v>
       </c>
       <c r="L23" s="1">
-        <f>($B23+1)^alpha / ($B23+L$2+$C23+1)^beta</f>
-        <v>0.43309035202934076</v>
+        <f>($B23+1)^alpha / ($B23+L$2*$R$4+$C23+1)^beta</f>
+        <v>1.3017082387567794E-11</v>
       </c>
       <c r="M23" s="1">
-        <f>($B23+1)^alpha / ($B23+M$2+$C23+1)^beta</f>
-        <v>0.41096889880084098</v>
+        <f>($B23+1)^alpha / ($B23+M$2*$R$4+$C23+1)^beta</f>
+        <v>8.0658290822293934E-12</v>
       </c>
       <c r="N23" s="1">
-        <f>($B23+1)^alpha / ($B23+N$2+$C23+1)^beta</f>
-        <v>0.39036703549100099</v>
+        <f>($B23+1)^alpha / ($B23+N$2*$R$4+$C23+1)^beta</f>
+        <v>5.2114129201546373E-12</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -3611,51 +3641,52 @@
         <v>44</v>
       </c>
       <c r="C24" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D24" s="1">
-        <f>($B24+1)^alpha / ($B24+D$2+$C24+1)^beta</f>
-        <v>0.68340593899316804</v>
+        <f>($B24+1)^alpha / ($B24+D$2*$R$4+$C24+1)^beta</f>
+        <v>3.6353287242794937E-8</v>
       </c>
       <c r="E24" s="1">
-        <f>($B24+1)^alpha / ($B24+E$2+$C24+1)^beta</f>
-        <v>0.64403043342854871</v>
+        <f>($B24+1)^alpha / ($B24+E$2*$R$4+$C24+1)^beta</f>
+        <v>4.9685795025359601E-9</v>
       </c>
       <c r="F24" s="1">
-        <f>($B24+1)^alpha / ($B24+F$2+$C24+1)^beta</f>
-        <v>0.60769871691967825</v>
+        <f>($B24+1)^alpha / ($B24+F$2*$R$4+$C24+1)^beta</f>
+        <v>1.2013131295908181E-9</v>
       </c>
       <c r="G24" s="1">
-        <f>($B24+1)^alpha / ($B24+G$2+$C24+1)^beta</f>
-        <v>0.5741180418123436</v>
+        <f>($B24+1)^alpha / ($B24+G$2*$R$4+$C24+1)^beta</f>
+        <v>3.9809925326293978E-10</v>
       </c>
       <c r="H24" s="1">
-        <f>($B24+1)^alpha / ($B24+H$2+$C24+1)^beta</f>
-        <v>0.54302912054174501</v>
+        <f>($B24+1)^alpha / ($B24+H$2*$R$4+$C24+1)^beta</f>
+        <v>1.6119369553203056E-10</v>
       </c>
       <c r="I24" s="1">
-        <f>($B24+1)^alpha / ($B24+I$2+$C24+1)^beta</f>
-        <v>0.51420171892060484</v>
+        <f>($B24+1)^alpha / ($B24+I$2*$R$4+$C24+1)^beta</f>
+        <v>7.4980402262009041E-11</v>
       </c>
       <c r="J24" s="1">
-        <f>($B24+1)^alpha / ($B24+J$2+$C24+1)^beta</f>
-        <v>0.48743090352300472</v>
+        <f>($B24+1)^alpha / ($B24+J$2*$R$4+$C24+1)^beta</f>
+        <v>3.8613567252660141E-11</v>
       </c>
       <c r="K24" s="1">
-        <f>($B24+1)^alpha / ($B24+K$2+$C24+1)^beta</f>
-        <v>0.4625338355465769</v>
+        <f>($B24+1)^alpha / ($B24+K$2*$R$4+$C24+1)^beta</f>
+        <v>2.1495169536956902E-11</v>
       </c>
       <c r="L24" s="1">
-        <f>($B24+1)^alpha / ($B24+L$2+$C24+1)^beta</f>
-        <v>0.43934702290963223</v>
+        <f>($B24+1)^alpha / ($B24+L$2*$R$4+$C24+1)^beta</f>
+        <v>1.2724621955897575E-11</v>
       </c>
       <c r="M24" s="1">
-        <f>($B24+1)^alpha / ($B24+M$2+$C24+1)^beta</f>
-        <v>0.41772395793666922</v>
+        <f>($B24+1)^alpha / ($B24+M$2*$R$4+$C24+1)^beta</f>
+        <v>7.917259665404074E-12</v>
       </c>
       <c r="N24" s="1">
-        <f>($B24+1)^alpha / ($B24+N$2+$C24+1)^beta</f>
-        <v>0.39753308059618986</v>
+        <f>($B24+1)^alpha / ($B24+N$2*$R$4+$C24+1)^beta</f>
+        <v>5.1330664589438755E-12</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -3667,51 +3698,52 @@
         <v>46</v>
       </c>
       <c r="C25" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D25" s="1">
-        <f>($B25+1)^alpha / ($B25+D$2+$C25+1)^beta</f>
-        <v>0.68044059271095747</v>
+        <f>($B25+1)^alpha / ($B25+D$2*$R$4+$C25+1)^beta</f>
+        <v>2.9892321136954355E-8</v>
       </c>
       <c r="E25" s="1">
-        <f>($B25+1)^alpha / ($B25+E$2+$C25+1)^beta</f>
-        <v>0.64284029203977966</v>
+        <f>($B25+1)^alpha / ($B25+E$2*$R$4+$C25+1)^beta</f>
+        <v>4.3833230099795418E-9</v>
       </c>
       <c r="F25" s="1">
-        <f>($B25+1)^alpha / ($B25+F$2+$C25+1)^beta</f>
-        <v>0.60803000953114239</v>
+        <f>($B25+1)^alpha / ($B25+F$2*$R$4+$C25+1)^beta</f>
+        <v>1.0986060019876761E-9</v>
       </c>
       <c r="G25" s="1">
-        <f>($B25+1)^alpha / ($B25+G$2+$C25+1)^beta</f>
-        <v>0.57575195183697414</v>
+        <f>($B25+1)^alpha / ($B25+G$2*$R$4+$C25+1)^beta</f>
+        <v>3.7209746521479938E-10</v>
       </c>
       <c r="H25" s="1">
-        <f>($B25+1)^alpha / ($B25+H$2+$C25+1)^beta</f>
-        <v>0.54577665488582661</v>
+        <f>($B25+1)^alpha / ($B25+H$2*$R$4+$C25+1)^beta</f>
+        <v>1.5289035409654088E-10</v>
       </c>
       <c r="I25" s="1">
-        <f>($B25+1)^alpha / ($B25+I$2+$C25+1)^beta</f>
-        <v>0.51789939396858053</v>
+        <f>($B25+1)^alpha / ($B25+I$2*$R$4+$C25+1)^beta</f>
+        <v>7.1870500113568406E-11</v>
       </c>
       <c r="J25" s="1">
-        <f>($B25+1)^alpha / ($B25+J$2+$C25+1)^beta</f>
-        <v>0.49193710691006448</v>
+        <f>($B25+1)^alpha / ($B25+J$2*$R$4+$C25+1)^beta</f>
+        <v>3.7306437078068333E-11</v>
       </c>
       <c r="K25" s="1">
-        <f>($B25+1)^alpha / ($B25+K$2+$C25+1)^beta</f>
-        <v>0.46772574898420077</v>
+        <f>($B25+1)^alpha / ($B25+K$2*$R$4+$C25+1)^beta</f>
+        <v>2.0896263780109643E-11</v>
       </c>
       <c r="L25" s="1">
-        <f>($B25+1)^alpha / ($B25+L$2+$C25+1)^beta</f>
-        <v>0.44511801235024978</v>
+        <f>($B25+1)^alpha / ($B25+L$2*$R$4+$C25+1)^beta</f>
+        <v>1.2431530897993464E-11</v>
       </c>
       <c r="M25" s="1">
-        <f>($B25+1)^alpha / ($B25+M$2+$C25+1)^beta</f>
-        <v>0.42398135425163769</v>
+        <f>($B25+1)^alpha / ($B25+M$2*$R$4+$C25+1)^beta</f>
+        <v>7.7663776911241313E-12</v>
       </c>
       <c r="N25" s="1">
-        <f>($B25+1)^alpha / ($B25+N$2+$C25+1)^beta</f>
-        <v>0.40419628756352449</v>
+        <f>($B25+1)^alpha / ($B25+N$2*$R$4+$C25+1)^beta</f>
+        <v>5.052340618807899E-12</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -3723,51 +3755,52 @@
         <v>48</v>
       </c>
       <c r="C26" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D26" s="1">
-        <f>($B26+1)^alpha / ($B26+D$2+$C26+1)^beta</f>
-        <v>0.67761091340048019</v>
+        <f>($B26+1)^alpha / ($B26+D$2*$R$4+$C26+1)^beta</f>
+        <v>2.4780932222490048E-8</v>
       </c>
       <c r="E26" s="1">
-        <f>($B26+1)^alpha / ($B26+E$2+$C26+1)^beta</f>
-        <v>0.64163906363305778</v>
+        <f>($B26+1)^alpha / ($B26+E$2*$R$4+$C26+1)^beta</f>
+        <v>3.8797728216316997E-9</v>
       </c>
       <c r="F26" s="1">
-        <f>($B26+1)^alpha / ($B26+F$2+$C26+1)^beta</f>
-        <v>0.60823349478263178</v>
+        <f>($B26+1)^alpha / ($B26+F$2*$R$4+$C26+1)^beta</f>
+        <v>1.0061976466623099E-9</v>
       </c>
       <c r="G26" s="1">
-        <f>($B26+1)^alpha / ($B26+G$2+$C26+1)^beta</f>
-        <v>0.57716605413475186</v>
+        <f>($B26+1)^alpha / ($B26+G$2*$R$4+$C26+1)^beta</f>
+        <v>3.4802371470880281E-10</v>
       </c>
       <c r="H26" s="1">
-        <f>($B26+1)^alpha / ($B26+H$2+$C26+1)^beta</f>
-        <v>0.54823273049624899</v>
+        <f>($B26+1)^alpha / ($B26+H$2*$R$4+$C26+1)^beta</f>
+        <v>1.4504247576641873E-10</v>
       </c>
       <c r="I26" s="1">
-        <f>($B26+1)^alpha / ($B26+I$2+$C26+1)^beta</f>
-        <v>0.52125070641579085</v>
+        <f>($B26+1)^alpha / ($B26+I$2*$R$4+$C26+1)^beta</f>
+        <v>6.888305791028675E-11</v>
       </c>
       <c r="J26" s="1">
-        <f>($B26+1)^alpha / ($B26+J$2+$C26+1)^beta</f>
-        <v>0.49605581664010062</v>
+        <f>($B26+1)^alpha / ($B26+J$2*$R$4+$C26+1)^beta</f>
+        <v>3.6033393605536137E-11</v>
       </c>
       <c r="K26" s="1">
-        <f>($B26+1)^alpha / ($B26+K$2+$C26+1)^beta</f>
-        <v>0.4725003506665077</v>
+        <f>($B26+1)^alpha / ($B26+K$2*$R$4+$C26+1)^beta</f>
+        <v>2.0305694618248362E-11</v>
       </c>
       <c r="L26" s="1">
-        <f>($B26+1)^alpha / ($B26+L$2+$C26+1)^beta</f>
-        <v>0.45045114766654443</v>
+        <f>($B26+1)^alpha / ($B26+L$2*$R$4+$C26+1)^beta</f>
+        <v>1.2139070941082829E-11</v>
       </c>
       <c r="M26" s="1">
-        <f>($B26+1)^alpha / ($B26+M$2+$C26+1)^beta</f>
-        <v>0.42978794057689951</v>
+        <f>($B26+1)^alpha / ($B26+M$2*$R$4+$C26+1)^beta</f>
+        <v>7.6140070344535117E-12</v>
       </c>
       <c r="N26" s="1">
-        <f>($B26+1)^alpha / ($B26+N$2+$C26+1)^beta</f>
-        <v>0.4104019131529088</v>
+        <f>($B26+1)^alpha / ($B26+N$2*$R$4+$C26+1)^beta</f>
+        <v>4.9697740036630793E-12</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -3779,51 +3812,52 @@
         <v>50</v>
       </c>
       <c r="C27" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D27" s="1">
-        <f>($B27+1)^alpha / ($B27+D$2+$C27+1)^beta</f>
-        <v>0.67490552337743748</v>
+        <f>($B27+1)^alpha / ($B27+D$2*$R$4+$C27+1)^beta</f>
+        <v>2.0698277612564798E-8</v>
       </c>
       <c r="E27" s="1">
-        <f>($B27+1)^alpha / ($B27+E$2+$C27+1)^beta</f>
-        <v>0.64043259896549243</v>
+        <f>($B27+1)^alpha / ($B27+E$2*$R$4+$C27+1)^beta</f>
+        <v>3.4448537390878475E-9</v>
       </c>
       <c r="F27" s="1">
-        <f>($B27+1)^alpha / ($B27+F$2+$C27+1)^beta</f>
-        <v>0.6083277246026112</v>
+        <f>($B27+1)^alpha / ($B27+F$2*$R$4+$C27+1)^beta</f>
+        <v>9.2292638425754063E-10</v>
       </c>
       <c r="G27" s="1">
-        <f>($B27+1)^alpha / ($B27+G$2+$C27+1)^beta</f>
-        <v>0.57838804314802084</v>
+        <f>($B27+1)^alpha / ($B27+G$2*$R$4+$C27+1)^beta</f>
+        <v>3.2572851498679879E-10</v>
       </c>
       <c r="H27" s="1">
-        <f>($B27+1)^alpha / ($B27+H$2+$C27+1)^beta</f>
-        <v>0.55043139423545817</v>
+        <f>($B27+1)^alpha / ($B27+H$2*$R$4+$C27+1)^beta</f>
+        <v>1.376293588722063E-10</v>
       </c>
       <c r="I27" s="1">
-        <f>($B27+1)^alpha / ($B27+I$2+$C27+1)^beta</f>
-        <v>0.5242938759506609</v>
+        <f>($B27+1)^alpha / ($B27+I$2*$R$4+$C27+1)^beta</f>
+        <v>6.6016988298575923E-11</v>
       </c>
       <c r="J27" s="1">
-        <f>($B27+1)^alpha / ($B27+J$2+$C27+1)^beta</f>
-        <v>0.49982773092840471</v>
+        <f>($B27+1)^alpha / ($B27+J$2*$R$4+$C27+1)^beta</f>
+        <v>3.479602541634079E-11</v>
       </c>
       <c r="K27" s="1">
-        <f>($B27+1)^alpha / ($B27+K$2+$C27+1)^beta</f>
-        <v>0.47689950892958655</v>
+        <f>($B27+1)^alpha / ($B27+K$2*$R$4+$C27+1)^beta</f>
+        <v>1.9724944175700292E-11</v>
       </c>
       <c r="L27" s="1">
-        <f>($B27+1)^alpha / ($B27+L$2+$C27+1)^beta</f>
-        <v>0.45538846572491465</v>
+        <f>($B27+1)^alpha / ($B27+L$2*$R$4+$C27+1)^beta</f>
+        <v>1.1848293453928942E-11</v>
       </c>
       <c r="M27" s="1">
-        <f>($B27+1)^alpha / ($B27+M$2+$C27+1)^beta</f>
-        <v>0.43518516451290462</v>
+        <f>($B27+1)^alpha / ($B27+M$2*$R$4+$C27+1)^beta</f>
+        <v>7.4608507552135507E-12</v>
       </c>
       <c r="N27" s="1">
-        <f>($B27+1)^alpha / ($B27+N$2+$C27+1)^beta</f>
-        <v>0.4161902513941097</v>
+        <f>($B27+1)^alpha / ($B27+N$2*$R$4+$C27+1)^beta</f>
+        <v>4.8858331706550357E-12</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -3835,51 +3869,52 @@
         <v>52</v>
       </c>
       <c r="C28" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D28" s="1">
-        <f>($B28+1)^alpha / ($B28+D$2+$C28+1)^beta</f>
-        <v>0.67231439957775063</v>
+        <f>($B28+1)^alpha / ($B28+D$2*$R$4+$C28+1)^beta</f>
+        <v>1.7408389165209195E-8</v>
       </c>
       <c r="E28" s="1">
-        <f>($B28+1)^alpha / ($B28+E$2+$C28+1)^beta</f>
-        <v>0.63922552634935847</v>
+        <f>($B28+1)^alpha / ($B28+E$2*$R$4+$C28+1)^beta</f>
+        <v>3.0678323154828189E-9</v>
       </c>
       <c r="F28" s="1">
-        <f>($B28+1)^alpha / ($B28+F$2+$C28+1)^beta</f>
-        <v>0.60832827003881673</v>
+        <f>($B28+1)^alpha / ($B28+F$2*$R$4+$C28+1)^beta</f>
+        <v>8.4777238020190374E-10</v>
       </c>
       <c r="G28" s="1">
-        <f>($B28+1)^alpha / ($B28+G$2+$C28+1)^beta</f>
-        <v>0.57944148878357271</v>
+        <f>($B28+1)^alpha / ($B28+G$2*$R$4+$C28+1)^beta</f>
+        <v>3.0507254694116002E-10</v>
       </c>
       <c r="H28" s="1">
-        <f>($B28+1)^alpha / ($B28+H$2+$C28+1)^beta</f>
-        <v>0.55240188342715801</v>
+        <f>($B28+1)^alpha / ($B28+H$2*$R$4+$C28+1)^beta</f>
+        <v>1.3062983296552388E-10</v>
       </c>
       <c r="I28" s="1">
-        <f>($B28+1)^alpha / ($B28+I$2+$C28+1)^beta</f>
-        <v>0.52706196682777795</v>
+        <f>($B28+1)^alpha / ($B28+I$2*$R$4+$C28+1)^beta</f>
+        <v>6.3270302780069004E-11</v>
       </c>
       <c r="J28" s="1">
-        <f>($B28+1)^alpha / ($B28+J$2+$C28+1)^beta</f>
-        <v>0.50328829432931099</v>
+        <f>($B28+1)^alpha / ($B28+J$2*$R$4+$C28+1)^beta</f>
+        <v>3.3595359500032078E-11</v>
       </c>
       <c r="K28" s="1">
-        <f>($B28+1)^alpha / ($B28+K$2+$C28+1)^beta</f>
-        <v>0.4809599180700932</v>
+        <f>($B28+1)^alpha / ($B28+K$2*$R$4+$C28+1)^beta</f>
+        <v>1.9155178682986172E-11</v>
       </c>
       <c r="L28" s="1">
-        <f>($B28+1)^alpha / ($B28+L$2+$C28+1)^beta</f>
-        <v>0.45996703365596187</v>
+        <f>($B28+1)^alpha / ($B28+L$2*$R$4+$C28+1)^beta</f>
+        <v>1.1560071576148503E-11</v>
       </c>
       <c r="M28" s="1">
-        <f>($B28+1)^alpha / ($B28+M$2+$C28+1)^beta</f>
-        <v>0.44020979257958059</v>
+        <f>($B28+1)^alpha / ($B28+M$2*$R$4+$C28+1)^beta</f>
+        <v>7.307508469707434E-12</v>
       </c>
       <c r="N28" s="1">
-        <f>($B28+1)^alpha / ($B28+N$2+$C28+1)^beta</f>
-        <v>0.42159725781010382</v>
+        <f>($B28+1)^alpha / ($B28+N$2*$R$4+$C28+1)^beta</f>
+        <v>4.8009225472008313E-12</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -3891,51 +3926,52 @@
         <v>54</v>
       </c>
       <c r="C29" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D29" s="1">
-        <f>($B29+1)^alpha / ($B29+D$2+$C29+1)^beta</f>
-        <v>0.66982866811966113</v>
+        <f>($B29+1)^alpha / ($B29+D$2*$R$4+$C29+1)^beta</f>
+        <v>1.4735602485365581E-8</v>
       </c>
       <c r="E29" s="1">
-        <f>($B29+1)^alpha / ($B29+E$2+$C29+1)^beta</f>
-        <v>0.63802150878243458</v>
+        <f>($B29+1)^alpha / ($B29+E$2*$R$4+$C29+1)^beta</f>
+        <v>2.7398558795006509E-9</v>
       </c>
       <c r="F29" s="1">
-        <f>($B29+1)^alpha / ($B29+F$2+$C29+1)^beta</f>
-        <v>0.60824826999934656</v>
+        <f>($B29+1)^alpha / ($B29+F$2*$R$4+$C29+1)^beta</f>
+        <v>7.798397562493428E-10</v>
       </c>
       <c r="G29" s="1">
-        <f>($B29+1)^alpha / ($B29+G$2+$C29+1)^beta</f>
-        <v>0.5803465540640621</v>
+        <f>($B29+1)^alpha / ($B29+G$2*$R$4+$C29+1)^beta</f>
+        <v>2.8592655597771789E-10</v>
       </c>
       <c r="H29" s="1">
-        <f>($B29+1)^alpha / ($B29+H$2+$C29+1)^beta</f>
-        <v>0.55416942541451741</v>
+        <f>($B29+1)^alpha / ($B29+H$2*$R$4+$C29+1)^beta</f>
+        <v>1.2402269303964103E-10</v>
       </c>
       <c r="I29" s="1">
-        <f>($B29+1)^alpha / ($B29+I$2+$C29+1)^beta</f>
-        <v>0.52958370867636184</v>
+        <f>($B29+1)^alpha / ($B29+I$2*$R$4+$C29+1)^beta</f>
+        <v>6.0640339445948893E-11</v>
       </c>
       <c r="J29" s="1">
-        <f>($B29+1)^alpha / ($B29+J$2+$C29+1)^beta</f>
-        <v>0.50646849851818465</v>
+        <f>($B29+1)^alpha / ($B29+J$2*$R$4+$C29+1)^beta</f>
+        <v>3.2431968688936589E-11</v>
       </c>
       <c r="K29" s="1">
-        <f>($B29+1)^alpha / ($B29+K$2+$C29+1)^beta</f>
-        <v>0.48471385200953715</v>
+        <f>($B29+1)^alpha / ($B29+K$2*$R$4+$C29+1)^beta</f>
+        <v>1.8597300740708445E-11</v>
       </c>
       <c r="L29" s="1">
-        <f>($B29+1)^alpha / ($B29+L$2+$C29+1)^beta</f>
-        <v>0.46421963862344223</v>
+        <f>($B29+1)^alpha / ($B29+L$2*$R$4+$C29+1)^beta</f>
+        <v>1.1275127076134366E-11</v>
       </c>
       <c r="M29" s="1">
-        <f>($B29+1)^alpha / ($B29+M$2+$C29+1)^beta</f>
-        <v>0.44489452674193325</v>
+        <f>($B29+1)^alpha / ($B29+M$2*$R$4+$C29+1)^beta</f>
+        <v>7.1544909534447495E-12</v>
       </c>
       <c r="N29" s="1">
-        <f>($B29+1)^alpha / ($B29+N$2+$C29+1)^beta</f>
-        <v>0.42665508863615059</v>
+        <f>($B29+1)^alpha / ($B29+N$2*$R$4+$C29+1)^beta</f>
+        <v>4.7153927953169862E-12</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -3947,51 +3983,52 @@
         <v>56</v>
       </c>
       <c r="C30" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D30" s="1">
-        <f>($B30+1)^alpha / ($B30+D$2+$C30+1)^beta</f>
-        <v>0.66744043624217186</v>
+        <f>($B30+1)^alpha / ($B30+D$2*$R$4+$C30+1)^beta</f>
+        <v>1.2547671765709797E-8</v>
       </c>
       <c r="E30" s="1">
-        <f>($B30+1)^alpha / ($B30+E$2+$C30+1)^beta</f>
-        <v>0.63682344253371237</v>
+        <f>($B30+1)^alpha / ($B30+E$2*$R$4+$C30+1)^beta</f>
+        <v>2.4535898782109877E-9</v>
       </c>
       <c r="F30" s="1">
-        <f>($B30+1)^alpha / ($B30+F$2+$C30+1)^beta</f>
-        <v>0.60809886570024529</v>
+        <f>($B30+1)^alpha / ($B30+F$2*$R$4+$C30+1)^beta</f>
+        <v>7.1834084122719941E-10</v>
       </c>
       <c r="G30" s="1">
-        <f>($B30+1)^alpha / ($B30+G$2+$C30+1)^beta</f>
-        <v>0.5811205702994896</v>
+        <f>($B30+1)^alpha / ($B30+G$2*$R$4+$C30+1)^beta</f>
+        <v>2.6817103653694172E-10</v>
       </c>
       <c r="H30" s="1">
-        <f>($B30+1)^alpha / ($B30+H$2+$C30+1)^beta</f>
-        <v>0.55575588500113304</v>
+        <f>($B30+1)^alpha / ($B30+H$2*$R$4+$C30+1)^beta</f>
+        <v>1.1778701521239204E-10</v>
       </c>
       <c r="I30" s="1">
-        <f>($B30+1)^alpha / ($B30+I$2+$C30+1)^beta</f>
-        <v>0.53188416769063163</v>
+        <f>($B30+1)^alpha / ($B30+I$2*$R$4+$C30+1)^beta</f>
+        <v>5.8123943521145787E-11</v>
       </c>
       <c r="J30" s="1">
-        <f>($B30+1)^alpha / ($B30+J$2+$C30+1)^beta</f>
-        <v>0.50939554355879468</v>
+        <f>($B30+1)^alpha / ($B30+J$2*$R$4+$C30+1)^beta</f>
+        <v>3.1306059546622584E-11</v>
       </c>
       <c r="K30" s="1">
-        <f>($B30+1)^alpha / ($B30+K$2+$C30+1)^beta</f>
-        <v>0.48818979297830062</v>
+        <f>($B30+1)^alpha / ($B30+K$2*$R$4+$C30+1)^beta</f>
+        <v>1.8051992788240728E-11</v>
       </c>
       <c r="L30" s="1">
-        <f>($B30+1)^alpha / ($B30+L$2+$C30+1)^beta</f>
-        <v>0.46817536938421667</v>
+        <f>($B30+1)^alpha / ($B30+L$2*$R$4+$C30+1)^beta</f>
+        <v>1.0994052909619213E-11</v>
       </c>
       <c r="M30" s="1">
-        <f>($B30+1)^alpha / ($B30+M$2+$C30+1)^beta</f>
-        <v>0.44926853024511365</v>
+        <f>($B30+1)^alpha / ($B30+M$2*$R$4+$C30+1)^beta</f>
+        <v>7.0022324809109118E-12</v>
       </c>
       <c r="N30" s="1">
-        <f>($B30+1)^alpha / ($B30+N$2+$C30+1)^beta</f>
-        <v>0.43139256662846093</v>
+        <f>($B30+1)^alpha / ($B30+N$2*$R$4+$C30+1)^beta</f>
+        <v>4.629547906328524E-12</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -4003,51 +4040,52 @@
         <v>58</v>
       </c>
       <c r="C31" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D31" s="1">
-        <f>($B31+1)^alpha / ($B31+D$2+$C31+1)^beta</f>
-        <v>0.66514265376588477</v>
+        <f>($B31+1)^alpha / ($B31+D$2*$R$4+$C31+1)^beta</f>
+        <v>1.0743998712328852E-8</v>
       </c>
       <c r="E31" s="1">
-        <f>($B31+1)^alpha / ($B31+E$2+$C31+1)^beta</f>
-        <v>0.635633611718462</v>
+        <f>($B31+1)^alpha / ($B31+E$2*$R$4+$C31+1)^beta</f>
+        <v>2.2029310862081628E-9</v>
       </c>
       <c r="F31" s="1">
-        <f>($B31+1)^alpha / ($B31+F$2+$C31+1)^beta</f>
-        <v>0.60788954731890454</v>
+        <f>($B31+1)^alpha / ($B31+F$2*$R$4+$C31+1)^beta</f>
+        <v>6.62582379624653E-10</v>
       </c>
       <c r="G31" s="1">
-        <f>($B31+1)^alpha / ($B31+G$2+$C31+1)^beta</f>
-        <v>0.5817785014060467</v>
+        <f>($B31+1)^alpha / ($B31+G$2*$R$4+$C31+1)^beta</f>
+        <v>2.5169578386615852E-10</v>
       </c>
       <c r="H31" s="1">
-        <f>($B31+1)^alpha / ($B31+H$2+$C31+1)^beta</f>
-        <v>0.55718029217017062</v>
+        <f>($B31+1)^alpha / ($B31+H$2*$R$4+$C31+1)^beta</f>
+        <v>1.11902382227513E-10</v>
       </c>
       <c r="I31" s="1">
-        <f>($B31+1)^alpha / ($B31+I$2+$C31+1)^beta</f>
-        <v>0.53398529870481515</v>
+        <f>($B31+1)^alpha / ($B31+I$2*$R$4+$C31+1)^beta</f>
+        <v>5.5717610463067933E-11</v>
       </c>
       <c r="J31" s="1">
-        <f>($B31+1)^alpha / ($B31+J$2+$C31+1)^beta</f>
-        <v>0.51209338675784277</v>
+        <f>($B31+1)^alpha / ($B31+J$2*$R$4+$C31+1)^beta</f>
+        <v>3.0217544446856245E-11</v>
       </c>
       <c r="K31" s="1">
-        <f>($B31+1)^alpha / ($B31+K$2+$C31+1)^beta</f>
-        <v>0.49141295818176528</v>
+        <f>($B31+1)^alpha / ($B31+K$2*$R$4+$C31+1)^beta</f>
+        <v>1.7519753387167855E-11</v>
       </c>
       <c r="L31" s="1">
-        <f>($B31+1)^alpha / ($B31+L$2+$C31+1)^beta</f>
-        <v>0.47186010822715962</v>
+        <f>($B31+1)^alpha / ($B31+L$2*$R$4+$C31+1)^beta</f>
+        <v>1.071733224747271E-11</v>
       </c>
       <c r="M31" s="1">
-        <f>($B31+1)^alpha / ($B31+M$2+$C31+1)^beta</f>
-        <v>0.45335787705616931</v>
+        <f>($B31+1)^alpha / ($B31+M$2*$R$4+$C31+1)^beta</f>
+        <v>6.8511013022694759E-12</v>
       </c>
       <c r="N31" s="1">
-        <f>($B31+1)^alpha / ($B31+N$2+$C31+1)^beta</f>
-        <v>0.43583558374426762</v>
+        <f>($B31+1)^alpha / ($B31+N$2*$R$4+$C31+1)^beta</f>
+        <v>4.5436512493683723E-12</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -4059,51 +4097,52 @@
         <v>60</v>
       </c>
       <c r="C32" s="2">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D32" s="1">
-        <f>($B32+1)^alpha / ($B32+D$2+$C32+1)^beta</f>
-        <v>0.66292899807937511</v>
+        <f>($B32+1)^alpha / ($B32+D$2*$R$4+$C32+1)^beta</f>
+        <v>9.2473169331423033E-9</v>
       </c>
       <c r="E32" s="1">
-        <f>($B32+1)^alpha / ($B32+E$2+$C32+1)^beta</f>
-        <v>0.6344538094827622</v>
+        <f>($B32+1)^alpha / ($B32+E$2*$R$4+$C32+1)^beta</f>
+        <v>1.9827796622982582E-9</v>
       </c>
       <c r="F32" s="1">
-        <f>($B32+1)^alpha / ($B32+F$2+$C32+1)^beta</f>
-        <v>0.60762843261091515</v>
+        <f>($B32+1)^alpha / ($B32+F$2*$R$4+$C32+1)^beta</f>
+        <v>6.1195349877246647E-10</v>
       </c>
       <c r="G32" s="1">
-        <f>($B32+1)^alpha / ($B32+G$2+$C32+1)^beta</f>
-        <v>0.5823333212765216</v>
+        <f>($B32+1)^alpha / ($B32+G$2*$R$4+$C32+1)^beta</f>
+        <v>2.3639936885783042E-10</v>
       </c>
       <c r="H32" s="1">
-        <f>($B32+1)^alpha / ($B32+H$2+$C32+1)^beta</f>
-        <v>0.55845927488592828</v>
+        <f>($B32+1)^alpha / ($B32+H$2*$R$4+$C32+1)^beta</f>
+        <v>1.0634904037017029E-10</v>
       </c>
       <c r="I32" s="1">
-        <f>($B32+1)^alpha / ($B32+I$2+$C32+1)^beta</f>
-        <v>0.53590640182492966</v>
+        <f>($B32+1)^alpha / ($B32+I$2*$R$4+$C32+1)^beta</f>
+        <v>5.3417599242697233E-11</v>
       </c>
       <c r="J32" s="1">
-        <f>($B32+1)^alpha / ($B32+J$2+$C32+1)^beta</f>
-        <v>0.51458320045196215</v>
+        <f>($B32+1)^alpha / ($B32+J$2*$R$4+$C32+1)^beta</f>
+        <v>2.9166100803685974E-11</v>
       </c>
       <c r="K32" s="1">
-        <f>($B32+1)^alpha / ($B32+K$2+$C32+1)^beta</f>
-        <v>0.49440574284224464</v>
+        <f>($B32+1)^alpha / ($B32+K$2*$R$4+$C32+1)^beta</f>
+        <v>1.7000927601757738E-11</v>
       </c>
       <c r="L32" s="1">
-        <f>($B32+1)^alpha / ($B32+L$2+$C32+1)^beta</f>
-        <v>0.47529694848882231</v>
+        <f>($B32+1)^alpha / ($B32+L$2*$R$4+$C32+1)^beta</f>
+        <v>1.044535458589108E-11</v>
       </c>
       <c r="M32" s="1">
-        <f>($B32+1)^alpha / ($B32+M$2+$C32+1)^beta</f>
-        <v>0.45718593691748555</v>
+        <f>($B32+1)^alpha / ($B32+M$2*$R$4+$C32+1)^beta</f>
+        <v>6.7014085759533707E-12</v>
       </c>
       <c r="N32" s="1">
-        <f>($B32+1)^alpha / ($B32+N$2+$C32+1)^beta</f>
-        <v>0.44000744966297539</v>
+        <f>($B32+1)^alpha / ($B32+N$2*$R$4+$C32+1)^beta</f>
+        <v>4.4579307516723526E-12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>